<commit_message>
rekonfiguration des Produktionslayouts gestartet, überarbeitung "convert_dict_to_machine.py" order und material list müssen noch überarbeitet werden
</commit_message>
<xml_diff>
--- a/analysis_solution/machine_statistics/Machine_data.xlsx
+++ b/analysis_solution/machine_statistics/Machine_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,16 +499,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.1</t>
+          <t>ProductGroup.FOURTEEN.1</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D2" t="n">
         <v>8</v>
@@ -520,16 +520,16 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I2" t="n">
-        <v>196</v>
+        <v>256</v>
       </c>
       <c r="J2" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -541,16 +541,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.2</t>
+          <t>ProductGroup.ELEVEN.3</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
@@ -562,16 +562,16 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>56.5</v>
+        <v>42</v>
       </c>
       <c r="H3" t="n">
-        <v>41.81805830021284</v>
+        <v>41.59326868617084</v>
       </c>
       <c r="I3" t="n">
-        <v>1748.75</v>
+        <v>1730</v>
       </c>
       <c r="J3" t="n">
-        <v>19</v>
+        <v>597</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -583,16 +583,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.3</t>
+          <t>ProductGroup.THREE.3</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
@@ -604,16 +604,16 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="H4" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="I4" t="n">
-        <v>256</v>
+        <v>1369</v>
       </c>
       <c r="J4" t="n">
-        <v>19</v>
+        <v>394</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -625,16 +625,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 1, 1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.3</t>
+          <t>ProductGroup.SEVEN.1</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>180</v>
+        <v>564</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
@@ -646,40 +646,40 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>34</v>
+        <v>23.42857142857143</v>
       </c>
       <c r="H5" t="n">
-        <v>24.37211521390788</v>
+        <v>9.663734014450149</v>
       </c>
       <c r="I5" t="n">
-        <v>594</v>
+        <v>93.38775510204081</v>
       </c>
       <c r="J5" t="n">
-        <v>782</v>
+        <v>497.5714285714286</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>798.1546318393014</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>637050.8163265308</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.3</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>92</v>
+        <v>564</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -688,22 +688,22 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>14</v>
+        <v>53.25</v>
       </c>
       <c r="H6" t="n">
-        <v>14</v>
+        <v>20.17269193736919</v>
       </c>
       <c r="I6" t="n">
-        <v>196</v>
+        <v>406.9375</v>
       </c>
       <c r="J6" t="n">
-        <v>917</v>
+        <v>46.66666666666666</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>1.885618083164127</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>3.555555555555556</v>
       </c>
     </row>
     <row r="7">
@@ -751,19 +751,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.4</t>
+          <t>ProductGroup.TWELVE.3</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -772,40 +772,40 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>18</v>
+        <v>16.5</v>
       </c>
       <c r="H8" t="n">
-        <v>18</v>
+        <v>16.87453703068621</v>
       </c>
       <c r="I8" t="n">
-        <v>324</v>
+        <v>284.75</v>
       </c>
       <c r="J8" t="n">
-        <v>94</v>
+        <v>475.5</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>441.5</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>194922.25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.4</t>
+          <t>ProductGroup.THREE.1</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -814,16 +814,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H9" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I9" t="n">
-        <v>121</v>
+        <v>361</v>
       </c>
       <c r="J9" t="n">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -835,19 +835,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.4</t>
+          <t>ProductGroup.TEN.1</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -856,16 +856,16 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H10" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I10" t="n">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="J10" t="n">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -877,19 +877,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.4</t>
+          <t>ProductGroup.ELEVEN.1</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -898,40 +898,40 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>36</v>
+        <v>14.5</v>
       </c>
       <c r="H11" t="n">
-        <v>36</v>
+        <v>14.51723114095797</v>
       </c>
       <c r="I11" t="n">
-        <v>1296</v>
+        <v>210.75</v>
       </c>
       <c r="J11" t="n">
-        <v>94</v>
+        <v>10210.5</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>10210.5</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>104254310.25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.4</t>
+          <t>ProductGroup.FOURTEEN.3</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -940,41 +940,41 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6</v>
+        <v>17.5</v>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>17.62810256380419</v>
       </c>
       <c r="I12" t="n">
-        <v>36</v>
+        <v>310.75</v>
       </c>
       <c r="J12" t="n">
-        <v>89</v>
+        <v>141.5</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>122.5</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>15006.25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.4</t>
+          <t>ProductGroup.TWO.3</t>
         </is>
       </c>
       <c r="C13" t="n">
+        <v>256</v>
+      </c>
+      <c r="D13" t="n">
         <v>8</v>
       </c>
-      <c r="D13" t="n">
-        <v>10</v>
-      </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
@@ -982,40 +982,40 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H13" t="n">
-        <v>6</v>
+        <v>23.93741840717165</v>
       </c>
       <c r="I13" t="n">
-        <v>36</v>
+        <v>573</v>
       </c>
       <c r="J13" t="n">
-        <v>94</v>
+        <v>411</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>371</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>137641</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.4</t>
+          <t>ProductGroup.FOUR.1</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1024,16 +1024,16 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H14" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I14" t="n">
-        <v>36</v>
+        <v>196</v>
       </c>
       <c r="J14" t="n">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1045,19 +1045,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.4</t>
+          <t>ProductGroup.SEVEN.3</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>84</v>
+        <v>356</v>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1066,41 +1066,41 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H15" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I15" t="n">
-        <v>121</v>
+        <v>256</v>
       </c>
       <c r="J15" t="n">
-        <v>227</v>
+        <v>304.8333333333333</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>439.8243651984531</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>193445.4722222222</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.4</t>
+          <t>ProductGroup.ONE.2</t>
         </is>
       </c>
       <c r="C16" t="n">
+        <v>48</v>
+      </c>
+      <c r="D16" t="n">
         <v>8</v>
       </c>
-      <c r="D16" t="n">
-        <v>10</v>
-      </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
@@ -1108,37 +1108,37 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>10</v>
+        <v>42.66666666666666</v>
       </c>
       <c r="H16" t="n">
-        <v>10</v>
+        <v>40.29336863003087</v>
       </c>
       <c r="I16" t="n">
-        <v>100</v>
+        <v>1623.555555555556</v>
       </c>
       <c r="J16" t="n">
-        <v>336</v>
+        <v>23.5</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.4</t>
+          <t>ProductGroup.SEVEN.1</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>12</v>
+        <v>356</v>
       </c>
       <c r="D17" t="n">
         <v>10</v>
@@ -1150,40 +1150,40 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H17" t="n">
-        <v>10</v>
+        <v>16.04992211819111</v>
       </c>
       <c r="I17" t="n">
-        <v>100</v>
+        <v>257.6</v>
       </c>
       <c r="J17" t="n">
-        <v>49</v>
+        <v>229.25</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>350.3094168017754</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>122716.6875</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ma: 1, 1</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.1</t>
+          <t>ProductGroup.THIRTEEN.3</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>564</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1192,37 +1192,37 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>23.42857142857143</v>
+        <v>11</v>
       </c>
       <c r="H18" t="n">
-        <v>9.663734014450149</v>
+        <v>11</v>
       </c>
       <c r="I18" t="n">
-        <v>93.38775510204081</v>
+        <v>121</v>
       </c>
       <c r="J18" t="n">
-        <v>497.5714285714286</v>
+        <v>567</v>
       </c>
       <c r="K18" t="n">
-        <v>798.1546318393014</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>637050.8163265308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.1</t>
+          <t>ProductGroup.EIGHT.1</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D19" t="n">
         <v>10</v>
@@ -1234,16 +1234,16 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I19" t="n">
-        <v>289</v>
+        <v>324</v>
       </c>
       <c r="J19" t="n">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -1255,16 +1255,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.1</t>
+          <t>ProductGroup.ONE.1</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="D20" t="n">
         <v>10</v>
@@ -1276,16 +1276,16 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H20" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I20" t="n">
-        <v>256</v>
+        <v>441</v>
       </c>
       <c r="J20" t="n">
-        <v>2078</v>
+        <v>46</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
@@ -1297,16 +1297,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.1</t>
+          <t>ProductGroup.NINE.3</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D21" t="n">
         <v>10</v>
@@ -1318,16 +1318,16 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H21" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I21" t="n">
-        <v>289</v>
+        <v>361</v>
       </c>
       <c r="J21" t="n">
-        <v>28</v>
+        <v>540</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -1339,16 +1339,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.3</t>
+          <t>ProductGroup.THREE.2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>564</v>
+        <v>84</v>
       </c>
       <c r="D22" t="n">
         <v>10</v>
@@ -1360,16 +1360,16 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>25.33333333333333</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>17.91337179005921</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>320.8888888888889</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>42</v>
+        <v>1870</v>
       </c>
       <c r="K22" t="n">
         <v>0</v>
@@ -1381,16 +1381,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.4</t>
+          <t>ProductGroup.FOUR.3</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="D23" t="n">
         <v>10</v>
@@ -1402,22 +1402,22 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>43.5</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>25.15452245621053</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>632.75</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>43.5</v>
+        <v>178</v>
       </c>
       <c r="K23" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1428,11 +1428,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.2</t>
+          <t>ProductGroup.TEN.3</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D24" t="n">
         <v>10</v>
@@ -1444,16 +1444,16 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>441</v>
       </c>
       <c r="J24" t="n">
-        <v>1870</v>
+        <v>53</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
@@ -1465,16 +1465,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.3</t>
+          <t>ProductGroup.THREE.1</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D25" t="n">
         <v>10</v>
@@ -1486,16 +1486,16 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H25" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I25" t="n">
-        <v>361</v>
+        <v>256</v>
       </c>
       <c r="J25" t="n">
-        <v>540</v>
+        <v>2078</v>
       </c>
       <c r="K25" t="n">
         <v>0</v>
@@ -1507,16 +1507,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.3</t>
+          <t>ProductGroup.TEN.1</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D26" t="n">
         <v>10</v>
@@ -1528,16 +1528,16 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H26" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I26" t="n">
-        <v>121</v>
+        <v>289</v>
       </c>
       <c r="J26" t="n">
-        <v>567</v>
+        <v>42</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
@@ -1549,16 +1549,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.3</t>
+          <t>ProductGroup.SEVEN.3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>52</v>
+        <v>564</v>
       </c>
       <c r="D27" t="n">
         <v>10</v>
@@ -1570,16 +1570,16 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>25.33333333333333</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>17.91337179005921</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>320.8888888888889</v>
       </c>
       <c r="J27" t="n">
-        <v>178</v>
+        <v>42</v>
       </c>
       <c r="K27" t="n">
         <v>0</v>
@@ -1591,16 +1591,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.1</t>
+          <t>ProductGroup.ELEVEN.1</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D28" t="n">
         <v>10</v>
@@ -1612,16 +1612,16 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H28" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I28" t="n">
-        <v>324</v>
+        <v>289</v>
       </c>
       <c r="J28" t="n">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="K28" t="n">
         <v>0</v>
@@ -1633,16 +1633,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.1</t>
+          <t>ProductGroup.TEN.4</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D29" t="n">
         <v>10</v>
@@ -1654,16 +1654,16 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>21</v>
+        <v>39.33333333333334</v>
       </c>
       <c r="H29" t="n">
-        <v>21</v>
+        <v>27.82484900627894</v>
       </c>
       <c r="I29" t="n">
-        <v>441</v>
+        <v>774.2222222222223</v>
       </c>
       <c r="J29" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
@@ -1675,16 +1675,16 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.3</t>
+          <t>ProductGroup.THIRTEEN.4</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D30" t="n">
         <v>10</v>
@@ -1696,16 +1696,16 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="H30" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I30" t="n">
-        <v>441</v>
+        <v>144</v>
       </c>
       <c r="J30" t="n">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
@@ -1717,12 +1717,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.1</t>
+          <t>ProductGroup.TWO.4</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1738,40 +1738,40 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>22</v>
+        <v>43.5</v>
       </c>
       <c r="H31" t="n">
-        <v>15.57776192739723</v>
+        <v>25.15452245621053</v>
       </c>
       <c r="I31" t="n">
-        <v>242.6666666666667</v>
+        <v>632.75</v>
       </c>
       <c r="J31" t="n">
-        <v>28</v>
+        <v>43.5</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.1</t>
+          <t>ProductGroup.FIFTEEN.4</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D32" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1780,16 +1780,16 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H32" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I32" t="n">
-        <v>256</v>
+        <v>196</v>
       </c>
       <c r="J32" t="n">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
@@ -1801,19 +1801,19 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.3</t>
+          <t>ProductGroup.EIGHT.4</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>24</v>
       </c>
       <c r="D33" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1822,16 +1822,16 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H33" t="n">
-        <v>41.59326868617084</v>
+        <v>14</v>
       </c>
       <c r="I33" t="n">
-        <v>1730</v>
+        <v>196</v>
       </c>
       <c r="J33" t="n">
-        <v>597</v>
+        <v>44</v>
       </c>
       <c r="K33" t="n">
         <v>0</v>
@@ -1843,37 +1843,37 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.3</t>
+          <t>ProductGroup.ONE.4</t>
         </is>
       </c>
       <c r="C34" t="n">
+        <v>16</v>
+      </c>
+      <c r="D34" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>79.33333333333333</v>
+      </c>
+      <c r="H34" t="n">
+        <v>70.84882183604435</v>
+      </c>
+      <c r="I34" t="n">
+        <v>5019.555555555556</v>
+      </c>
+      <c r="J34" t="n">
         <v>84</v>
-      </c>
-      <c r="D34" t="n">
-        <v>8</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="n">
-        <v>37</v>
-      </c>
-      <c r="H34" t="n">
-        <v>37</v>
-      </c>
-      <c r="I34" t="n">
-        <v>1369</v>
-      </c>
-      <c r="J34" t="n">
-        <v>394</v>
       </c>
       <c r="K34" t="n">
         <v>0</v>
@@ -1885,16 +1885,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.3</t>
+          <t>ProductGroup.TWELVE.4</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D35" t="n">
         <v>10</v>
@@ -1906,16 +1906,16 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>62.8</v>
+        <v>52.5</v>
       </c>
       <c r="H35" t="n">
-        <v>65.61219398861769</v>
+        <v>34.24543765233553</v>
       </c>
       <c r="I35" t="n">
-        <v>4304.96</v>
+        <v>1172.75</v>
       </c>
       <c r="J35" t="n">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="K35" t="n">
         <v>0</v>
@@ -1927,16 +1927,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.1</t>
+          <t>ProductGroup.TEN.4</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D36" t="n">
         <v>10</v>
@@ -1957,7 +1957,7 @@
         <v>324</v>
       </c>
       <c r="J36" t="n">
-        <v>172</v>
+        <v>94</v>
       </c>
       <c r="K36" t="n">
         <v>0</v>
@@ -1969,16 +1969,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.2</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>52</v>
+        <v>356</v>
       </c>
       <c r="D37" t="n">
         <v>10</v>
@@ -1990,37 +1990,37 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H37" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="I37" t="n">
-        <v>144</v>
+        <v>900</v>
       </c>
       <c r="J37" t="n">
-        <v>3407</v>
+        <v>46.75</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>1.299038105676658</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>1.6875</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.2</t>
+          <t>ProductGroup.THREE.4</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="D38" t="n">
         <v>10</v>
@@ -2032,16 +2032,16 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>24.66666666666667</v>
+        <v>11</v>
       </c>
       <c r="H38" t="n">
-        <v>17.46106780494506</v>
+        <v>11</v>
       </c>
       <c r="I38" t="n">
-        <v>304.8888888888889</v>
+        <v>121</v>
       </c>
       <c r="J38" t="n">
-        <v>1795</v>
+        <v>227</v>
       </c>
       <c r="K38" t="n">
         <v>0</v>
@@ -2053,16 +2053,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.3</t>
+          <t>ProductGroup.FOURTEEN.4</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D39" t="n">
         <v>10</v>
@@ -2074,33 +2074,33 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H39" t="n">
-        <v>15</v>
+        <v>8.246211251235321</v>
       </c>
       <c r="I39" t="n">
-        <v>225</v>
+        <v>68</v>
       </c>
       <c r="J39" t="n">
-        <v>207</v>
+        <v>304.5</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>216.5</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>46872.25</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.3</t>
+          <t>ProductGroup.THIRTEEN.4</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -2116,16 +2116,16 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H40" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I40" t="n">
-        <v>324</v>
+        <v>36</v>
       </c>
       <c r="J40" t="n">
-        <v>611</v>
+        <v>94</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
@@ -2137,16 +2137,16 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.4</t>
+          <t>ProductGroup.TWO.4</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>564</v>
+        <v>76</v>
       </c>
       <c r="D41" t="n">
         <v>10</v>
@@ -2158,22 +2158,862 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>53.25</v>
+        <v>33</v>
       </c>
       <c r="H41" t="n">
-        <v>20.17269193736919</v>
+        <v>33</v>
       </c>
       <c r="I41" t="n">
-        <v>406.9375</v>
+        <v>1089</v>
       </c>
       <c r="J41" t="n">
-        <v>46.66666666666666</v>
+        <v>87</v>
       </c>
       <c r="K41" t="n">
-        <v>1.885618083164127</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>3.555555555555556</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Ma: 0, 4</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ProductGroup.FIFTEEN.4</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>8</v>
+      </c>
+      <c r="D42" t="n">
+        <v>10</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>10</v>
+      </c>
+      <c r="H42" t="n">
+        <v>10</v>
+      </c>
+      <c r="I42" t="n">
+        <v>100</v>
+      </c>
+      <c r="J42" t="n">
+        <v>336</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Ma: 0, 4</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ProductGroup.ONE.4</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>32</v>
+      </c>
+      <c r="D43" t="n">
+        <v>10</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>36</v>
+      </c>
+      <c r="H43" t="n">
+        <v>36</v>
+      </c>
+      <c r="I43" t="n">
+        <v>1296</v>
+      </c>
+      <c r="J43" t="n">
+        <v>94</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Ma: 0, 4</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ProductGroup.EIGHT.4</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>12</v>
+      </c>
+      <c r="D44" t="n">
+        <v>10</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>10</v>
+      </c>
+      <c r="H44" t="n">
+        <v>10</v>
+      </c>
+      <c r="I44" t="n">
+        <v>100</v>
+      </c>
+      <c r="J44" t="n">
+        <v>49</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Ma: 0, 4</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ProductGroup.NINE.4</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>104</v>
+      </c>
+      <c r="D45" t="n">
+        <v>10</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H45" t="n">
+        <v>6.538348415311011</v>
+      </c>
+      <c r="I45" t="n">
+        <v>42.75</v>
+      </c>
+      <c r="J45" t="n">
+        <v>174.5</v>
+      </c>
+      <c r="K45" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="L45" t="n">
+        <v>7482.25</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Ma: 0, 4</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ProductGroup.ELEVEN.4</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>24</v>
+      </c>
+      <c r="D46" t="n">
+        <v>10</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>11</v>
+      </c>
+      <c r="H46" t="n">
+        <v>11</v>
+      </c>
+      <c r="I46" t="n">
+        <v>121</v>
+      </c>
+      <c r="J46" t="n">
+        <v>89</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Ma: 0, 4</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOUR.4</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>52</v>
+      </c>
+      <c r="D47" t="n">
+        <v>10</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>6</v>
+      </c>
+      <c r="H47" t="n">
+        <v>6</v>
+      </c>
+      <c r="I47" t="n">
+        <v>36</v>
+      </c>
+      <c r="J47" t="n">
+        <v>89</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ProductGroup.FIFTEEN.3</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>12</v>
+      </c>
+      <c r="D48" t="n">
+        <v>10</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="H48" t="n">
+        <v>18.51350858157362</v>
+      </c>
+      <c r="I48" t="n">
+        <v>342.75</v>
+      </c>
+      <c r="J48" t="n">
+        <v>322.5</v>
+      </c>
+      <c r="K48" t="n">
+        <v>288.5</v>
+      </c>
+      <c r="L48" t="n">
+        <v>83232.25</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ProductGroup.THIRTEEN.1</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>20</v>
+      </c>
+      <c r="D49" t="n">
+        <v>10</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>18</v>
+      </c>
+      <c r="H49" t="n">
+        <v>18</v>
+      </c>
+      <c r="I49" t="n">
+        <v>324</v>
+      </c>
+      <c r="J49" t="n">
+        <v>592</v>
+      </c>
+      <c r="K49" t="n">
+        <v>420</v>
+      </c>
+      <c r="L49" t="n">
+        <v>176400</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ProductGroup.TWO.2</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>256</v>
+      </c>
+      <c r="D50" t="n">
+        <v>10</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>22</v>
+      </c>
+      <c r="H50" t="n">
+        <v>17.97776404339539</v>
+      </c>
+      <c r="I50" t="n">
+        <v>323.2</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1014.5</v>
+      </c>
+      <c r="K50" t="n">
+        <v>780.5</v>
+      </c>
+      <c r="L50" t="n">
+        <v>609180.25</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ProductGroup.EIGHT.3</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>36</v>
+      </c>
+      <c r="D51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>20.4</v>
+      </c>
+      <c r="H51" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="I51" t="n">
+        <v>282.24</v>
+      </c>
+      <c r="J51" t="n">
+        <v>117</v>
+      </c>
+      <c r="K51" t="n">
+        <v>90</v>
+      </c>
+      <c r="L51" t="n">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOURTEEN.1</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>16</v>
+      </c>
+      <c r="D52" t="n">
+        <v>10</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>20</v>
+      </c>
+      <c r="H52" t="n">
+        <v>20</v>
+      </c>
+      <c r="I52" t="n">
+        <v>400</v>
+      </c>
+      <c r="J52" t="n">
+        <v>630</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ProductGroup.ONE.3</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>48</v>
+      </c>
+      <c r="D53" t="n">
+        <v>10</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>72.48275862068965</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1249.998384519549</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1562495.961301481</v>
+      </c>
+      <c r="J53" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K53" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L53" t="n">
+        <v>72.25</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOUR.2</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>52</v>
+      </c>
+      <c r="D54" t="n">
+        <v>10</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>12</v>
+      </c>
+      <c r="H54" t="n">
+        <v>12</v>
+      </c>
+      <c r="I54" t="n">
+        <v>144</v>
+      </c>
+      <c r="J54" t="n">
+        <v>3407</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ProductGroup.THIRTEEN.3</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>12</v>
+      </c>
+      <c r="D55" t="n">
+        <v>10</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>11</v>
+      </c>
+      <c r="H55" t="n">
+        <v>11</v>
+      </c>
+      <c r="I55" t="n">
+        <v>121</v>
+      </c>
+      <c r="J55" t="n">
+        <v>449</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ProductGroup.EIGHT.1</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>24</v>
+      </c>
+      <c r="D56" t="n">
+        <v>10</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>16</v>
+      </c>
+      <c r="H56" t="n">
+        <v>16</v>
+      </c>
+      <c r="I56" t="n">
+        <v>256</v>
+      </c>
+      <c r="J56" t="n">
+        <v>501</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>ProductGroup.TWO.1</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>256</v>
+      </c>
+      <c r="D57" t="n">
+        <v>10</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>62.4</v>
+      </c>
+      <c r="H57" t="n">
+        <v>92.98085824512485</v>
+      </c>
+      <c r="I57" t="n">
+        <v>8645.440000000001</v>
+      </c>
+      <c r="J57" t="n">
+        <v>105</v>
+      </c>
+      <c r="K57" t="n">
+        <v>77</v>
+      </c>
+      <c r="L57" t="n">
+        <v>5929</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ProductGroup.ONE.1</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>16</v>
+      </c>
+      <c r="D58" t="n">
+        <v>10</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>16</v>
+      </c>
+      <c r="H58" t="n">
+        <v>16</v>
+      </c>
+      <c r="I58" t="n">
+        <v>256</v>
+      </c>
+      <c r="J58" t="n">
+        <v>2664</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ProductGroup.NINE.3</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>60</v>
+      </c>
+      <c r="D59" t="n">
+        <v>10</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>16</v>
+      </c>
+      <c r="H59" t="n">
+        <v>16</v>
+      </c>
+      <c r="I59" t="n">
+        <v>256</v>
+      </c>
+      <c r="J59" t="n">
+        <v>783</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ProductGroup.THREE.2</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>36</v>
+      </c>
+      <c r="D60" t="n">
+        <v>10</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>18</v>
+      </c>
+      <c r="H60" t="n">
+        <v>18</v>
+      </c>
+      <c r="I60" t="n">
+        <v>324</v>
+      </c>
+      <c r="J60" t="n">
+        <v>10</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ProductGroup.TEN.3</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>44</v>
+      </c>
+      <c r="D61" t="n">
+        <v>10</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>24</v>
+      </c>
+      <c r="H61" t="n">
+        <v>16.97056274847714</v>
+      </c>
+      <c r="I61" t="n">
+        <v>288</v>
+      </c>
+      <c r="J61" t="n">
+        <v>38</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2255,11 +3095,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>396</v>
+        <v>148</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -2271,32 +3111,32 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>32.14285714285715</v>
+        <v>34.25</v>
       </c>
       <c r="G2" t="n">
-        <v>32.6143201301364</v>
+        <v>37.23489626680864</v>
       </c>
       <c r="H2" t="n">
-        <v>1063.69387755102</v>
+        <v>1386.4375</v>
       </c>
       <c r="I2" t="n">
-        <v>351.2</v>
+        <v>338</v>
       </c>
       <c r="J2" t="n">
-        <v>409.0938278683755</v>
+        <v>237.6566150282097</v>
       </c>
       <c r="K2" t="n">
-        <v>167357.76</v>
+        <v>56480.66666666666</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ma: 0, 1</t>
+          <t>Ma: 1, 1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>92</v>
+        <v>564</v>
       </c>
       <c r="C3" t="n">
         <v>8</v>
@@ -2308,32 +3148,32 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>9</v>
+        <v>23.42857142857143</v>
       </c>
       <c r="G3" t="n">
-        <v>9</v>
+        <v>9.663734014450149</v>
       </c>
       <c r="H3" t="n">
-        <v>81</v>
+        <v>93.38775510204081</v>
       </c>
       <c r="I3" t="n">
-        <v>43</v>
+        <v>497.5714285714286</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>798.1546318393014</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>637050.8163265308</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>356</v>
+        <v>564</v>
       </c>
       <c r="C4" t="n">
         <v>10</v>
@@ -2345,32 +3185,32 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>12.4</v>
+        <v>53.25</v>
       </c>
       <c r="G4" t="n">
-        <v>17.32743489383239</v>
+        <v>20.17269193736919</v>
       </c>
       <c r="H4" t="n">
-        <v>300.2400000000001</v>
+        <v>406.9375</v>
       </c>
       <c r="I4" t="n">
-        <v>124.8</v>
+        <v>46.66666666666666</v>
       </c>
       <c r="J4" t="n">
-        <v>83.01421565009211</v>
+        <v>1.885618083164127</v>
       </c>
       <c r="K4" t="n">
-        <v>6891.359999999999</v>
+        <v>3.555555555555556</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 1, 1</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>564</v>
+        <v>92</v>
       </c>
       <c r="C5" t="n">
         <v>8</v>
@@ -2382,35 +3222,35 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>23.42857142857143</v>
+        <v>9</v>
       </c>
       <c r="G5" t="n">
-        <v>9.663734014450149</v>
+        <v>9</v>
       </c>
       <c r="H5" t="n">
-        <v>93.38775510204081</v>
+        <v>81</v>
       </c>
       <c r="I5" t="n">
-        <v>497.5714285714286</v>
+        <v>43</v>
       </c>
       <c r="J5" t="n">
-        <v>798.1546318393014</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>637050.8163265308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>724</v>
+        <v>1060</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2419,32 +3259,32 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>19.55555555555556</v>
+        <v>25.58823529411765</v>
       </c>
       <c r="G6" t="n">
-        <v>17.58225817320221</v>
+        <v>26.7043922880497</v>
       </c>
       <c r="H6" t="n">
-        <v>309.1358024691358</v>
+        <v>713.1245674740485</v>
       </c>
       <c r="I6" t="n">
-        <v>547.5</v>
+        <v>1286.368421052632</v>
       </c>
       <c r="J6" t="n">
-        <v>883.6530710635254</v>
+        <v>4523.764433935481</v>
       </c>
       <c r="K6" t="n">
-        <v>780842.75</v>
+        <v>20464444.65373961</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>180</v>
+        <v>640</v>
       </c>
       <c r="C7" t="n">
         <v>10</v>
@@ -2456,32 +3296,32 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>43.5</v>
+        <v>20</v>
       </c>
       <c r="G7" t="n">
-        <v>25.15452245621053</v>
+        <v>19.34212105894344</v>
       </c>
       <c r="H7" t="n">
-        <v>632.75</v>
+        <v>374.1176470588235</v>
       </c>
       <c r="I7" t="n">
-        <v>43.5</v>
+        <v>389.9090909090909</v>
       </c>
       <c r="J7" t="n">
-        <v>1.5</v>
+        <v>538.4566251705727</v>
       </c>
       <c r="K7" t="n">
-        <v>2.25</v>
+        <v>289935.5371900826</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>284</v>
+        <v>724</v>
       </c>
       <c r="C8" t="n">
         <v>10</v>
@@ -2493,32 +3333,32 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>15</v>
+        <v>19.55555555555556</v>
       </c>
       <c r="G8" t="n">
-        <v>18.37570860311696</v>
+        <v>17.58225817320221</v>
       </c>
       <c r="H8" t="n">
-        <v>337.6666666666667</v>
+        <v>309.1358024691358</v>
       </c>
       <c r="I8" t="n">
-        <v>481.7142857142857</v>
+        <v>547.5</v>
       </c>
       <c r="J8" t="n">
-        <v>601.9232780455173</v>
+        <v>883.6530710635254</v>
       </c>
       <c r="K8" t="n">
-        <v>362311.6326530612</v>
+        <v>780842.75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>180</v>
+        <v>280</v>
       </c>
       <c r="C9" t="n">
         <v>10</v>
@@ -2530,35 +3370,35 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>22</v>
+        <v>38.125</v>
       </c>
       <c r="G9" t="n">
-        <v>15.57776192739723</v>
+        <v>43.22307688029625</v>
       </c>
       <c r="H9" t="n">
-        <v>242.6666666666667</v>
+        <v>1868.234375</v>
       </c>
       <c r="I9" t="n">
-        <v>28</v>
+        <v>65.28571428571429</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>37.59070662397551</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1413.061224489796</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>148</v>
+        <v>928</v>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -2567,22 +3407,22 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>34.25</v>
+        <v>18.8125</v>
       </c>
       <c r="G10" t="n">
-        <v>37.23489626680864</v>
+        <v>26.00413128235589</v>
       </c>
       <c r="H10" t="n">
-        <v>1386.4375</v>
+        <v>676.21484375</v>
       </c>
       <c r="I10" t="n">
-        <v>338</v>
+        <v>133.1111111111111</v>
       </c>
       <c r="J10" t="n">
-        <v>237.6566150282097</v>
+        <v>122.4912191360348</v>
       </c>
       <c r="K10" t="n">
-        <v>56480.66666666666</v>
+        <v>15004.0987654321</v>
       </c>
     </row>
     <row r="11">
@@ -2592,7 +3432,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>292</v>
+        <v>440</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
@@ -2604,32 +3444,32 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>32.125</v>
+        <v>69.04398826979472</v>
       </c>
       <c r="G11" t="n">
-        <v>44.39858528151544</v>
+        <v>1209.082954325467</v>
       </c>
       <c r="H11" t="n">
-        <v>1971.234375</v>
+        <v>1461881.590440399</v>
       </c>
       <c r="I11" t="n">
-        <v>1035</v>
+        <v>679</v>
       </c>
       <c r="J11" t="n">
-        <v>1214.386127500914</v>
+        <v>966.9947431777142</v>
       </c>
       <c r="K11" t="n">
-        <v>1474733.666666667</v>
+        <v>935078.8333333334</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>564</v>
+        <v>448</v>
       </c>
       <c r="C12" t="n">
         <v>10</v>
@@ -2641,22 +3481,22 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>53.25</v>
+        <v>29.88888888888889</v>
       </c>
       <c r="G12" t="n">
-        <v>20.17269193736919</v>
+        <v>54.80256369600168</v>
       </c>
       <c r="H12" t="n">
-        <v>406.9375</v>
+        <v>3003.320987654321</v>
       </c>
       <c r="I12" t="n">
-        <v>46.66666666666666</v>
+        <v>581.875</v>
       </c>
       <c r="J12" t="n">
-        <v>1.885618083164127</v>
+        <v>828.3576277037594</v>
       </c>
       <c r="K12" t="n">
-        <v>3.555555555555556</v>
+        <v>686176.359375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intermediate store komplett (auch monitoring & rebuilding )eingebaut
</commit_message>
<xml_diff>
--- a/analysis_solution/machine_statistics/Machine_data.xlsx
+++ b/analysis_solution/machine_statistics/Machine_data.xlsx
@@ -499,19 +499,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.1</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>36</v>
+        <v>564</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -520,40 +520,40 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>14</v>
+        <v>47.71428571428572</v>
       </c>
       <c r="H2" t="n">
-        <v>14</v>
+        <v>19.49149474378347</v>
       </c>
       <c r="I2" t="n">
-        <v>196</v>
+        <v>379.9183673469388</v>
       </c>
       <c r="J2" t="n">
-        <v>36</v>
+        <v>42.5</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1.118033988749895</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.3</t>
+          <t>ProductGroup.TEN.1</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>356</v>
+        <v>52</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -562,16 +562,16 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="H3" t="n">
-        <v>20.32240143290158</v>
+        <v>20</v>
       </c>
       <c r="I3" t="n">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="J3" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -583,19 +583,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.1</t>
+          <t>ProductGroup.THREE.1</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -604,16 +604,16 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H4" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I4" t="n">
-        <v>441</v>
+        <v>256</v>
       </c>
       <c r="J4" t="n">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -625,7 +625,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -634,10 +634,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -646,40 +646,40 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>27</v>
+        <v>49.2</v>
       </c>
       <c r="H5" t="n">
-        <v>27</v>
+        <v>31.6379518932563</v>
       </c>
       <c r="I5" t="n">
-        <v>729</v>
+        <v>1000.96</v>
       </c>
       <c r="J5" t="n">
-        <v>862.5</v>
+        <v>23</v>
       </c>
       <c r="K5" t="n">
-        <v>846.5</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>716562.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.1</t>
+          <t>ProductGroup.ELEVEN.1</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -688,16 +688,16 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H6" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I6" t="n">
-        <v>196</v>
+        <v>289</v>
       </c>
       <c r="J6" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -709,19 +709,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.3</t>
+          <t>ProductGroup.SEVEN.3</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>156</v>
+        <v>564</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -730,40 +730,40 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>17</v>
+        <v>35.23076923076923</v>
       </c>
       <c r="H7" t="n">
-        <v>17.52141546793523</v>
+        <v>10.18410410057561</v>
       </c>
       <c r="I7" t="n">
-        <v>307</v>
+        <v>103.7159763313609</v>
       </c>
       <c r="J7" t="n">
-        <v>1413</v>
+        <v>908</v>
       </c>
       <c r="K7" t="n">
-        <v>1176</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1382976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.3</t>
+          <t>ProductGroup.TWO.4</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -772,40 +772,40 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>44.33333333333334</v>
+        <v>30</v>
       </c>
       <c r="H8" t="n">
-        <v>38.80578421948059</v>
+        <v>30</v>
       </c>
       <c r="I8" t="n">
-        <v>1505.888888888889</v>
+        <v>900</v>
       </c>
       <c r="J8" t="n">
-        <v>132.5</v>
+        <v>49.5</v>
       </c>
       <c r="K8" t="n">
-        <v>111.5</v>
+        <v>1.5</v>
       </c>
       <c r="L8" t="n">
-        <v>12432.25</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.2</t>
+          <t>ProductGroup.THIRTEEN.4</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -814,40 +814,40 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>47.6</v>
+        <v>11</v>
       </c>
       <c r="H9" t="n">
-        <v>46.03303161861056</v>
+        <v>11</v>
       </c>
       <c r="I9" t="n">
-        <v>2119.04</v>
+        <v>121</v>
       </c>
       <c r="J9" t="n">
-        <v>5.5</v>
+        <v>249</v>
       </c>
       <c r="K9" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.1</t>
+          <t>ProductGroup.NINE.4</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -856,37 +856,37 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>13.5</v>
+        <v>11</v>
       </c>
       <c r="H10" t="n">
-        <v>13.51850583459577</v>
+        <v>11</v>
       </c>
       <c r="I10" t="n">
-        <v>182.75</v>
+        <v>121</v>
       </c>
       <c r="J10" t="n">
-        <v>20.5</v>
+        <v>48</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.1</t>
+          <t>ProductGroup.TEN.4</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D11" t="n">
         <v>8</v>
@@ -898,16 +898,16 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>16</v>
+        <v>51.33333333333334</v>
       </c>
       <c r="H11" t="n">
-        <v>16</v>
+        <v>38.86157771143912</v>
       </c>
       <c r="I11" t="n">
-        <v>256</v>
+        <v>1510.222222222222</v>
       </c>
       <c r="J11" t="n">
-        <v>256</v>
+        <v>82</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -919,16 +919,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.3</t>
+          <t>ProductGroup.EIGHT.4</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>564</v>
+        <v>24</v>
       </c>
       <c r="D12" t="n">
         <v>8</v>
@@ -940,16 +940,16 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>35.23076923076923</v>
+        <v>29.33333333333333</v>
       </c>
       <c r="H12" t="n">
-        <v>10.18410410057561</v>
+        <v>25.42090128658349</v>
       </c>
       <c r="I12" t="n">
-        <v>103.7159763313609</v>
+        <v>646.2222222222223</v>
       </c>
       <c r="J12" t="n">
-        <v>908</v>
+        <v>48</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
@@ -961,16 +961,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.1</t>
+          <t>ProductGroup.FOUR.4</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
@@ -982,16 +982,16 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H13" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I13" t="n">
-        <v>289</v>
+        <v>784</v>
       </c>
       <c r="J13" t="n">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1003,16 +1003,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.3</t>
+          <t>ProductGroup.ONE.4</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="D14" t="n">
         <v>8</v>
@@ -1024,16 +1024,16 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>49.2</v>
+        <v>87.33333333333333</v>
       </c>
       <c r="H14" t="n">
-        <v>31.6379518932563</v>
+        <v>85.82669877271421</v>
       </c>
       <c r="I14" t="n">
-        <v>1000.96</v>
+        <v>7366.222222222222</v>
       </c>
       <c r="J14" t="n">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1045,16 +1045,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.1</t>
+          <t>ProductGroup.FIFTEEN.4</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
         <v>8</v>
@@ -1066,16 +1066,16 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H15" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I15" t="n">
-        <v>400</v>
+        <v>784</v>
       </c>
       <c r="J15" t="n">
-        <v>42</v>
+        <v>290</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1087,16 +1087,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.1</t>
+          <t>ProductGroup.THREE.4</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D16" t="n">
         <v>8</v>
@@ -1108,16 +1108,16 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>18</v>
+        <v>42.66666666666666</v>
       </c>
       <c r="H16" t="n">
-        <v>18</v>
+        <v>30.5650490302604</v>
       </c>
       <c r="I16" t="n">
-        <v>324</v>
+        <v>934.2222222222223</v>
       </c>
       <c r="J16" t="n">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1129,16 +1129,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.3</t>
+          <t>ProductGroup.ELEVEN.4</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D17" t="n">
         <v>8</v>
@@ -1150,16 +1150,16 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H17" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I17" t="n">
-        <v>324</v>
+        <v>841</v>
       </c>
       <c r="J17" t="n">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -1171,16 +1171,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.3</t>
+          <t>ProductGroup.ONE.3</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D18" t="n">
         <v>8</v>
@@ -1192,37 +1192,37 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>26</v>
+        <v>69.25</v>
       </c>
       <c r="H18" t="n">
-        <v>26</v>
+        <v>66.67786364304123</v>
       </c>
       <c r="I18" t="n">
-        <v>676</v>
+        <v>4445.9375</v>
       </c>
       <c r="J18" t="n">
-        <v>131</v>
+        <v>35.5</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>30.25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.2</t>
+          <t>ProductGroup.ELEVEN.3</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D19" t="n">
         <v>8</v>
@@ -1234,37 +1234,37 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>17.95995545651492</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>322.5600000000001</v>
       </c>
       <c r="J19" t="n">
-        <v>274</v>
+        <v>37.5</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>90.25</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.3</t>
+          <t>ProductGroup.FOURTEEN.1</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D20" t="n">
         <v>8</v>
@@ -1276,16 +1276,16 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H20" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I20" t="n">
-        <v>576</v>
+        <v>441</v>
       </c>
       <c r="J20" t="n">
-        <v>59</v>
+        <v>545</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
@@ -1297,16 +1297,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.1</t>
+          <t>ProductGroup.FOUR.2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D21" t="n">
         <v>8</v>
@@ -1318,16 +1318,16 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H21" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I21" t="n">
-        <v>400</v>
+        <v>729</v>
       </c>
       <c r="J21" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -1339,16 +1339,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.1</t>
+          <t>ProductGroup.FIFTEEN.3</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>356</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
         <v>8</v>
@@ -1360,37 +1360,37 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>63.2</v>
+        <v>18.5</v>
       </c>
       <c r="H22" t="n">
-        <v>73.73031940796135</v>
+        <v>18.51350858157362</v>
       </c>
       <c r="I22" t="n">
-        <v>5436.160000000002</v>
+        <v>342.75</v>
       </c>
       <c r="J22" t="n">
-        <v>27.5</v>
+        <v>34.5</v>
       </c>
       <c r="K22" t="n">
-        <v>1.5</v>
+        <v>7.5</v>
       </c>
       <c r="L22" t="n">
-        <v>2.25</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.3</t>
+          <t>ProductGroup.THREE.3</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="D23" t="n">
         <v>8</v>
@@ -1402,37 +1402,37 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>19</v>
+        <v>39.4</v>
       </c>
       <c r="H23" t="n">
-        <v>19</v>
+        <v>26.68407764941483</v>
       </c>
       <c r="I23" t="n">
-        <v>361</v>
+        <v>712.04</v>
       </c>
       <c r="J23" t="n">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.1</t>
+          <t>ProductGroup.THIRTEEN.1</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D24" t="n">
         <v>8</v>
@@ -1444,37 +1444,37 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>16</v>
+        <v>18.5</v>
       </c>
       <c r="H24" t="n">
-        <v>16</v>
+        <v>18.51350858157362</v>
       </c>
       <c r="I24" t="n">
-        <v>256</v>
+        <v>342.75</v>
       </c>
       <c r="J24" t="n">
-        <v>33</v>
+        <v>180.5</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>71.5</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>5112.25</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.3</t>
+          <t>ProductGroup.EIGHT.3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D25" t="n">
         <v>8</v>
@@ -1486,33 +1486,33 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H25" t="n">
-        <v>24</v>
+        <v>30.7571129984594</v>
       </c>
       <c r="I25" t="n">
-        <v>576</v>
+        <v>946</v>
       </c>
       <c r="J25" t="n">
-        <v>623</v>
+        <v>29.5</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.1</t>
+          <t>ProductGroup.TWO.2</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1528,22 +1528,22 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>20.8</v>
+        <v>16.5</v>
       </c>
       <c r="H26" t="n">
-        <v>17.0926884953772</v>
+        <v>16.63580475961412</v>
       </c>
       <c r="I26" t="n">
-        <v>292.16</v>
+        <v>276.75</v>
       </c>
       <c r="J26" t="n">
-        <v>770.6666666666666</v>
+        <v>1010.666666666667</v>
       </c>
       <c r="K26" t="n">
-        <v>529.6648835715739</v>
+        <v>1237.400860226341</v>
       </c>
       <c r="L26" t="n">
-        <v>280544.8888888889</v>
+        <v>1531160.888888889</v>
       </c>
     </row>
     <row r="27">
@@ -1554,11 +1554,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.3</t>
+          <t>ProductGroup.ONE.1</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D27" t="n">
         <v>8</v>
@@ -1570,16 +1570,16 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H27" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I27" t="n">
-        <v>196</v>
+        <v>256</v>
       </c>
       <c r="J27" t="n">
-        <v>182</v>
+        <v>33</v>
       </c>
       <c r="K27" t="n">
         <v>0</v>
@@ -1596,11 +1596,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.2</t>
+          <t>ProductGroup.TEN.3</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D28" t="n">
         <v>8</v>
@@ -1612,16 +1612,16 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>28</v>
+        <v>24.4</v>
       </c>
       <c r="H28" t="n">
-        <v>16.18641405623865</v>
+        <v>15.56406116667497</v>
       </c>
       <c r="I28" t="n">
-        <v>262</v>
+        <v>242.24</v>
       </c>
       <c r="J28" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="K28" t="n">
         <v>0</v>
@@ -1638,11 +1638,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.3</t>
+          <t>ProductGroup.THIRTEEN.3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D29" t="n">
         <v>8</v>
@@ -1654,16 +1654,16 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="H29" t="n">
-        <v>48.68949236402724</v>
+        <v>14</v>
       </c>
       <c r="I29" t="n">
-        <v>2370.666666666667</v>
+        <v>196</v>
       </c>
       <c r="J29" t="n">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
@@ -1680,32 +1680,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.1</t>
+          <t>ProductGroup.NINE.3</t>
         </is>
       </c>
       <c r="C30" t="n">
+        <v>60</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
         <v>24</v>
       </c>
-      <c r="D30" t="n">
-        <v>8</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>17</v>
-      </c>
       <c r="H30" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I30" t="n">
-        <v>289</v>
+        <v>576</v>
       </c>
       <c r="J30" t="n">
-        <v>177</v>
+        <v>623</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
@@ -1722,11 +1722,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.3</t>
+          <t>ProductGroup.THREE.2</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D31" t="n">
         <v>8</v>
@@ -1738,16 +1738,16 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>24.4</v>
+        <v>28</v>
       </c>
       <c r="H31" t="n">
-        <v>15.56406116667497</v>
+        <v>16.18641405623865</v>
       </c>
       <c r="I31" t="n">
-        <v>242.24</v>
+        <v>262</v>
       </c>
       <c r="J31" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
@@ -1759,19 +1759,19 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.2</t>
+          <t>ProductGroup.EIGHT.1</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D32" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1780,16 +1780,16 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H32" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I32" t="n">
-        <v>169</v>
+        <v>289</v>
       </c>
       <c r="J32" t="n">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
@@ -1801,19 +1801,19 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.1</t>
+          <t>ProductGroup.FOUR.3</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1822,13 +1822,13 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="H33" t="n">
-        <v>17</v>
+        <v>48.68949236402724</v>
       </c>
       <c r="I33" t="n">
-        <v>289</v>
+        <v>2370.666666666667</v>
       </c>
       <c r="J33" t="n">
         <v>25</v>
@@ -1843,16 +1843,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.4</t>
+          <t>ProductGroup.TWO.1</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>564</v>
+        <v>256</v>
       </c>
       <c r="D34" t="n">
         <v>8</v>
@@ -1864,40 +1864,40 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>47.71428571428572</v>
+        <v>20.8</v>
       </c>
       <c r="H34" t="n">
-        <v>19.49149474378347</v>
+        <v>17.0926884953772</v>
       </c>
       <c r="I34" t="n">
-        <v>379.9183673469388</v>
+        <v>292.16</v>
       </c>
       <c r="J34" t="n">
-        <v>42.5</v>
+        <v>770.6666666666666</v>
       </c>
       <c r="K34" t="n">
-        <v>1.118033988749895</v>
+        <v>529.6648835715739</v>
       </c>
       <c r="L34" t="n">
-        <v>1.25</v>
+        <v>280544.8888888889</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ma: 0, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.4</t>
+          <t>ProductGroup.TWO.4</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D35" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -1906,16 +1906,16 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>30</v>
+        <v>38.66666666666666</v>
       </c>
       <c r="H35" t="n">
-        <v>30</v>
+        <v>27.34146220587984</v>
       </c>
       <c r="I35" t="n">
-        <v>900</v>
+        <v>747.5555555555555</v>
       </c>
       <c r="J35" t="n">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="K35" t="n">
         <v>0</v>
@@ -1927,16 +1927,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.3</t>
+          <t>ProductGroup.THIRTEEN.4</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="D36" t="n">
         <v>8</v>
@@ -1948,37 +1948,37 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>39.4</v>
+        <v>35</v>
       </c>
       <c r="H36" t="n">
-        <v>26.68407764941483</v>
+        <v>35</v>
       </c>
       <c r="I36" t="n">
-        <v>712.04</v>
+        <v>1225</v>
       </c>
       <c r="J36" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="K36" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>3249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.3</t>
+          <t>ProductGroup.TWELVE.4</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="D37" t="n">
         <v>8</v>
@@ -1990,37 +1990,37 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="H37" t="n">
-        <v>30.7571129984594</v>
+        <v>31.24099870362662</v>
       </c>
       <c r="I37" t="n">
-        <v>946</v>
+        <v>976</v>
       </c>
       <c r="J37" t="n">
-        <v>29.5</v>
+        <v>299</v>
       </c>
       <c r="K37" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.1</t>
+          <t>ProductGroup.FOURTEEN.4</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D38" t="n">
         <v>8</v>
@@ -2032,37 +2032,37 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>21</v>
+        <v>31.5</v>
       </c>
       <c r="H38" t="n">
-        <v>21</v>
+        <v>31.5079355083763</v>
       </c>
       <c r="I38" t="n">
-        <v>441</v>
+        <v>992.75</v>
       </c>
       <c r="J38" t="n">
-        <v>545</v>
+        <v>112</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>529</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.2</t>
+          <t>ProductGroup.NINE.4</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D39" t="n">
         <v>8</v>
@@ -2074,16 +2074,16 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H39" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I39" t="n">
-        <v>729</v>
+        <v>1024</v>
       </c>
       <c r="J39" t="n">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
@@ -2095,16 +2095,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.3</t>
+          <t>ProductGroup.TEN.4</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D40" t="n">
         <v>8</v>
@@ -2116,37 +2116,37 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>69.25</v>
+        <v>32</v>
       </c>
       <c r="H40" t="n">
-        <v>66.67786364304123</v>
+        <v>32</v>
       </c>
       <c r="I40" t="n">
-        <v>4445.9375</v>
+        <v>1024</v>
       </c>
       <c r="J40" t="n">
-        <v>35.5</v>
+        <v>88</v>
       </c>
       <c r="K40" t="n">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>30.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.2</t>
+          <t>ProductGroup.EIGHT.4</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>256</v>
+        <v>12</v>
       </c>
       <c r="D41" t="n">
         <v>8</v>
@@ -2158,37 +2158,37 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>16.5</v>
+        <v>32</v>
       </c>
       <c r="H41" t="n">
-        <v>16.63580475961412</v>
+        <v>32</v>
       </c>
       <c r="I41" t="n">
-        <v>276.75</v>
+        <v>1024</v>
       </c>
       <c r="J41" t="n">
-        <v>1010.666666666667</v>
+        <v>49</v>
       </c>
       <c r="K41" t="n">
-        <v>1237.400860226341</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>1531160.888888889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.1</t>
+          <t>ProductGroup.FOUR.4</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D42" t="n">
         <v>8</v>
@@ -2200,37 +2200,37 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>18.5</v>
+        <v>32</v>
       </c>
       <c r="H42" t="n">
-        <v>18.51350858157362</v>
+        <v>32</v>
       </c>
       <c r="I42" t="n">
-        <v>342.75</v>
+        <v>1024</v>
       </c>
       <c r="J42" t="n">
-        <v>180.5</v>
+        <v>88</v>
       </c>
       <c r="K42" t="n">
-        <v>71.5</v>
+        <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>5112.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.3</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>52</v>
+        <v>356</v>
       </c>
       <c r="D43" t="n">
         <v>8</v>
@@ -2242,37 +2242,37 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>19.2</v>
+        <v>48.33333333333334</v>
       </c>
       <c r="H43" t="n">
-        <v>17.95995545651492</v>
+        <v>21.67692065051881</v>
       </c>
       <c r="I43" t="n">
-        <v>322.5600000000001</v>
+        <v>469.8888888888889</v>
       </c>
       <c r="J43" t="n">
-        <v>37.5</v>
+        <v>46.5</v>
       </c>
       <c r="K43" t="n">
-        <v>9.5</v>
+        <v>0.8660254037844386</v>
       </c>
       <c r="L43" t="n">
-        <v>90.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.3</t>
+          <t>ProductGroup.ONE.4</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D44" t="n">
         <v>8</v>
@@ -2284,37 +2284,37 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>18.5</v>
+        <v>32</v>
       </c>
       <c r="H44" t="n">
-        <v>18.51350858157362</v>
+        <v>32</v>
       </c>
       <c r="I44" t="n">
-        <v>342.75</v>
+        <v>1024</v>
       </c>
       <c r="J44" t="n">
-        <v>34.5</v>
+        <v>89</v>
       </c>
       <c r="K44" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>56.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.4</t>
+          <t>ProductGroup.FIFTEEN.4</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="D45" t="n">
         <v>8</v>
@@ -2326,16 +2326,16 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>51.33333333333334</v>
+        <v>32</v>
       </c>
       <c r="H45" t="n">
-        <v>38.86157771143912</v>
+        <v>32</v>
       </c>
       <c r="I45" t="n">
-        <v>1510.222222222222</v>
+        <v>1024</v>
       </c>
       <c r="J45" t="n">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="K45" t="n">
         <v>0</v>
@@ -2347,16 +2347,16 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.4</t>
+          <t>ProductGroup.THREE.4</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
@@ -2368,37 +2368,37 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H46" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="I46" t="n">
-        <v>900</v>
+        <v>1681</v>
       </c>
       <c r="J46" t="n">
-        <v>49.5</v>
+        <v>184</v>
       </c>
       <c r="K46" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.4</t>
+          <t>ProductGroup.ELEVEN.4</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D47" t="n">
         <v>8</v>
@@ -2410,16 +2410,16 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="H47" t="n">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="I47" t="n">
-        <v>121</v>
+        <v>1369</v>
       </c>
       <c r="J47" t="n">
-        <v>249</v>
+        <v>89</v>
       </c>
       <c r="K47" t="n">
         <v>0</v>
@@ -2431,19 +2431,19 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.4</t>
+          <t>ProductGroup.TEN.1</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D48" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -2452,16 +2452,16 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>42.66666666666666</v>
+        <v>14</v>
       </c>
       <c r="H48" t="n">
-        <v>30.5650490302604</v>
+        <v>14</v>
       </c>
       <c r="I48" t="n">
-        <v>934.2222222222223</v>
+        <v>196</v>
       </c>
       <c r="J48" t="n">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="K48" t="n">
         <v>0</v>
@@ -2473,19 +2473,19 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.4</t>
+          <t>ProductGroup.FOUR.1</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="D49" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -2494,40 +2494,40 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>29.33333333333333</v>
+        <v>13.5</v>
       </c>
       <c r="H49" t="n">
-        <v>25.42090128658349</v>
+        <v>13.51850583459577</v>
       </c>
       <c r="I49" t="n">
-        <v>646.2222222222223</v>
+        <v>182.75</v>
       </c>
       <c r="J49" t="n">
-        <v>48</v>
+        <v>20.5</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L49" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.4</t>
+          <t>ProductGroup.TWELVE.3</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4</v>
+        <v>156</v>
       </c>
       <c r="D50" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -2536,40 +2536,40 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H50" t="n">
-        <v>28</v>
+        <v>17.52141546793523</v>
       </c>
       <c r="I50" t="n">
-        <v>784</v>
+        <v>307</v>
       </c>
       <c r="J50" t="n">
-        <v>290</v>
+        <v>1413</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>1176</v>
       </c>
       <c r="L50" t="n">
-        <v>0</v>
+        <v>1382976</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.4</t>
+          <t>ProductGroup.TWO.3</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="D51" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -2578,40 +2578,40 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H51" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="I51" t="n">
-        <v>121</v>
+        <v>729</v>
       </c>
       <c r="J51" t="n">
-        <v>48</v>
+        <v>862.5</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>846.5</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>716562.25</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.4</t>
+          <t>ProductGroup.ONE.2</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D52" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -2620,40 +2620,40 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>29</v>
+        <v>47.6</v>
       </c>
       <c r="H52" t="n">
-        <v>29</v>
+        <v>46.03303161861056</v>
       </c>
       <c r="I52" t="n">
-        <v>841</v>
+        <v>2119.04</v>
       </c>
       <c r="J52" t="n">
-        <v>82</v>
+        <v>5.5</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L52" t="n">
-        <v>0</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.4</t>
+          <t>ProductGroup.THREE.1</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D53" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -2662,16 +2662,16 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H53" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I53" t="n">
-        <v>784</v>
+        <v>196</v>
       </c>
       <c r="J53" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="K53" t="n">
         <v>0</v>
@@ -2683,19 +2683,19 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.4</t>
+          <t>ProductGroup.ELEVEN.1</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D54" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -2704,16 +2704,16 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>87.33333333333333</v>
+        <v>21</v>
       </c>
       <c r="H54" t="n">
-        <v>85.82669877271421</v>
+        <v>21</v>
       </c>
       <c r="I54" t="n">
-        <v>7366.222222222222</v>
+        <v>441</v>
       </c>
       <c r="J54" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="K54" t="n">
         <v>0</v>
@@ -2725,16 +2725,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Ma: 1, 1</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.1</t>
+          <t>ProductGroup.FOURTEEN.3</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>564</v>
+        <v>56</v>
       </c>
       <c r="D55" t="n">
         <v>10</v>
@@ -2746,40 +2746,40 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>22.57142857142857</v>
+        <v>44.33333333333334</v>
       </c>
       <c r="H55" t="n">
-        <v>9.240549502169273</v>
+        <v>38.80578421948059</v>
       </c>
       <c r="I55" t="n">
-        <v>85.38775510204081</v>
+        <v>1505.888888888889</v>
       </c>
       <c r="J55" t="n">
-        <v>19</v>
+        <v>132.5</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
+        <v>111.5</v>
       </c>
       <c r="L55" t="n">
-        <v>0</v>
+        <v>12432.25</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.4</t>
+          <t>ProductGroup.SEVEN.3</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>52</v>
+        <v>356</v>
       </c>
       <c r="D56" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -2788,16 +2788,16 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H56" t="n">
-        <v>32</v>
+        <v>20.32240143290158</v>
       </c>
       <c r="I56" t="n">
-        <v>1024</v>
+        <v>413</v>
       </c>
       <c r="J56" t="n">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K56" t="n">
         <v>0</v>
@@ -2809,19 +2809,19 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.4</t>
+          <t>ProductGroup.FOURTEEN.1</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D57" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -2830,16 +2830,16 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H57" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I57" t="n">
-        <v>1225</v>
+        <v>289</v>
       </c>
       <c r="J57" t="n">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="K57" t="n">
         <v>0</v>
@@ -2851,19 +2851,19 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.4</t>
+          <t>ProductGroup.FOUR.2</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D58" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>38.66666666666666</v>
+        <v>13</v>
       </c>
       <c r="H58" t="n">
-        <v>27.34146220587984</v>
+        <v>13</v>
       </c>
       <c r="I58" t="n">
-        <v>747.5555555555555</v>
+        <v>169</v>
       </c>
       <c r="J58" t="n">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="K58" t="n">
         <v>0</v>
@@ -2893,19 +2893,19 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.4</t>
+          <t>ProductGroup.TWELVE.4</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D59" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -2914,16 +2914,16 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H59" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I59" t="n">
-        <v>1681</v>
+        <v>900</v>
       </c>
       <c r="J59" t="n">
-        <v>184</v>
+        <v>44</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
@@ -2935,16 +2935,16 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.4</t>
+          <t>ProductGroup.ONE.1</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D60" t="n">
         <v>8</v>
@@ -2956,13 +2956,13 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H60" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="I60" t="n">
-        <v>1024</v>
+        <v>324</v>
       </c>
       <c r="J60" t="n">
         <v>49</v>
@@ -2977,16 +2977,16 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.4</t>
+          <t>ProductGroup.TEN.3</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>356</v>
+        <v>52</v>
       </c>
       <c r="D61" t="n">
         <v>8</v>
@@ -2998,33 +2998,33 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>48.33333333333334</v>
+        <v>19</v>
       </c>
       <c r="H61" t="n">
-        <v>21.67692065051881</v>
+        <v>19</v>
       </c>
       <c r="I61" t="n">
-        <v>469.8888888888889</v>
+        <v>361</v>
       </c>
       <c r="J61" t="n">
-        <v>46.5</v>
+        <v>48</v>
       </c>
       <c r="K61" t="n">
-        <v>0.8660254037844386</v>
+        <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.4</t>
+          <t>ProductGroup.THIRTEEN.3</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -3040,16 +3040,16 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H62" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I62" t="n">
-        <v>1024</v>
+        <v>676</v>
       </c>
       <c r="J62" t="n">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="K62" t="n">
         <v>0</v>
@@ -3061,12 +3061,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.4</t>
+          <t>ProductGroup.NINE.3</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -3082,16 +3082,16 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H63" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="I63" t="n">
-        <v>1024</v>
+        <v>324</v>
       </c>
       <c r="J63" t="n">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="K63" t="n">
         <v>0</v>
@@ -3103,16 +3103,16 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.4</t>
+          <t>ProductGroup.THREE.2</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="D64" t="n">
         <v>8</v>
@@ -3124,16 +3124,16 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>1369</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>89</v>
+        <v>274</v>
       </c>
       <c r="K64" t="n">
         <v>0</v>
@@ -3145,16 +3145,16 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.4</t>
+          <t>ProductGroup.EIGHT.1</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D65" t="n">
         <v>8</v>
@@ -3166,33 +3166,33 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>31.5</v>
+        <v>20</v>
       </c>
       <c r="H65" t="n">
-        <v>31.5079355083763</v>
+        <v>20</v>
       </c>
       <c r="I65" t="n">
-        <v>992.75</v>
+        <v>400</v>
       </c>
       <c r="J65" t="n">
-        <v>112</v>
+        <v>29</v>
       </c>
       <c r="K65" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="L65" t="n">
-        <v>529</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.4</t>
+          <t>ProductGroup.FOUR.3</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -3208,16 +3208,16 @@
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H66" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="I66" t="n">
-        <v>1024</v>
+        <v>576</v>
       </c>
       <c r="J66" t="n">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="K66" t="n">
         <v>0</v>
@@ -3229,16 +3229,16 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.4</t>
+          <t>ProductGroup.SEVEN.1</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="D67" t="n">
         <v>8</v>
@@ -3250,40 +3250,40 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>56</v>
+        <v>63.2</v>
       </c>
       <c r="H67" t="n">
-        <v>31.24099870362662</v>
+        <v>73.73031940796135</v>
       </c>
       <c r="I67" t="n">
-        <v>976</v>
+        <v>5436.160000000002</v>
       </c>
       <c r="J67" t="n">
-        <v>299</v>
+        <v>27.5</v>
       </c>
       <c r="K67" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L67" t="n">
-        <v>0</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 1</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.4</t>
+          <t>ProductGroup.SEVEN.1</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>32</v>
+        <v>564</v>
       </c>
       <c r="D68" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -3292,16 +3292,16 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>32</v>
+        <v>22.57142857142857</v>
       </c>
       <c r="H68" t="n">
-        <v>32</v>
+        <v>9.240549502169273</v>
       </c>
       <c r="I68" t="n">
-        <v>1024</v>
+        <v>85.38775510204081</v>
       </c>
       <c r="J68" t="n">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="K68" t="n">
         <v>0</v>
@@ -3389,14 +3389,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>972</v>
+        <v>564</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -3405,22 +3405,22 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>31.75757575757576</v>
+        <v>47.71428571428572</v>
       </c>
       <c r="G2" t="n">
-        <v>32.18792386296291</v>
+        <v>19.49149474378347</v>
       </c>
       <c r="H2" t="n">
-        <v>1036.062442607897</v>
+        <v>379.9183673469388</v>
       </c>
       <c r="I2" t="n">
-        <v>357.2142857142857</v>
+        <v>42.5</v>
       </c>
       <c r="J2" t="n">
-        <v>753.985712120351</v>
+        <v>1.118033988749895</v>
       </c>
       <c r="K2" t="n">
-        <v>568494.4540816328</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="3">
@@ -3463,11 +3463,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>640</v>
+        <v>420</v>
       </c>
       <c r="C4" t="n">
         <v>8</v>
@@ -3479,32 +3479,32 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>31.44444444444444</v>
+        <v>37.75</v>
       </c>
       <c r="G4" t="n">
-        <v>47.13953545028988</v>
+        <v>45.73588124583731</v>
       </c>
       <c r="H4" t="n">
-        <v>2222.135802469136</v>
+        <v>2091.770833333333</v>
       </c>
       <c r="I4" t="n">
-        <v>76.77777777777777</v>
+        <v>101.2727272727273</v>
       </c>
       <c r="J4" t="n">
-        <v>75.89726649707745</v>
+        <v>81.28411553321183</v>
       </c>
       <c r="K4" t="n">
-        <v>5760.395061728395</v>
+        <v>6607.107438016529</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>464</v>
+        <v>576</v>
       </c>
       <c r="C5" t="n">
         <v>8</v>
@@ -3516,35 +3516,35 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>25.68</v>
+        <v>34.09302325581395</v>
       </c>
       <c r="G5" t="n">
-        <v>25.79724016246699</v>
+        <v>40.15308725915506</v>
       </c>
       <c r="H5" t="n">
-        <v>665.4976000000001</v>
+        <v>1612.27041644132</v>
       </c>
       <c r="I5" t="n">
-        <v>341.4</v>
+        <v>261.1176470588235</v>
       </c>
       <c r="J5" t="n">
-        <v>437.5118741245773</v>
+        <v>637.4406438206335</v>
       </c>
       <c r="K5" t="n">
-        <v>191416.64</v>
+        <v>406330.5743944637</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92</v>
+        <v>464</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -3553,32 +3553,32 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>15</v>
+        <v>25.68</v>
       </c>
       <c r="G6" t="n">
-        <v>15.26433752247375</v>
+        <v>25.79724016246699</v>
       </c>
       <c r="H6" t="n">
-        <v>233</v>
+        <v>665.4975999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>29.5</v>
+        <v>341.4</v>
       </c>
       <c r="J6" t="n">
-        <v>4.5</v>
+        <v>437.5118741245773</v>
       </c>
       <c r="K6" t="n">
-        <v>20.25</v>
+        <v>191416.64</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>564</v>
+        <v>868</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
@@ -3590,32 +3590,32 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>47.71428571428572</v>
+        <v>39.94594594594594</v>
       </c>
       <c r="G7" t="n">
-        <v>19.49149474378347</v>
+        <v>32.38780713682563</v>
       </c>
       <c r="H7" t="n">
-        <v>379.9183673469388</v>
+        <v>1048.970051132213</v>
       </c>
       <c r="I7" t="n">
-        <v>42.5</v>
+        <v>98.76470588235294</v>
       </c>
       <c r="J7" t="n">
-        <v>1.118033988749895</v>
+        <v>61.01738364815748</v>
       </c>
       <c r="K7" t="n">
-        <v>1.25</v>
+        <v>3723.121107266436</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 0, 1</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>92</v>
+        <v>972</v>
       </c>
       <c r="C8" t="n">
         <v>10</v>
@@ -3627,35 +3627,35 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>30</v>
+        <v>31.75757575757576</v>
       </c>
       <c r="G8" t="n">
-        <v>30</v>
+        <v>32.18792386296292</v>
       </c>
       <c r="H8" t="n">
-        <v>900</v>
+        <v>1036.062442607898</v>
       </c>
       <c r="I8" t="n">
-        <v>44</v>
+        <v>357.2142857142857</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>753.9857121203509</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>568494.4540816327</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>576</v>
+        <v>92</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -3664,35 +3664,35 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>34.09302325581395</v>
+        <v>15</v>
       </c>
       <c r="G9" t="n">
-        <v>40.15308725915506</v>
+        <v>15.26433752247375</v>
       </c>
       <c r="H9" t="n">
-        <v>1612.27041644132</v>
+        <v>233</v>
       </c>
       <c r="I9" t="n">
-        <v>261.1176470588235</v>
+        <v>29.5</v>
       </c>
       <c r="J9" t="n">
-        <v>637.4406438206333</v>
+        <v>4.5</v>
       </c>
       <c r="K9" t="n">
-        <v>406330.5743944636</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>420</v>
+        <v>92</v>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -3701,35 +3701,35 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>37.75</v>
+        <v>30</v>
       </c>
       <c r="G10" t="n">
-        <v>45.73588124583731</v>
+        <v>30</v>
       </c>
       <c r="H10" t="n">
-        <v>2091.770833333333</v>
+        <v>900</v>
       </c>
       <c r="I10" t="n">
-        <v>101.2727272727273</v>
+        <v>44</v>
       </c>
       <c r="J10" t="n">
-        <v>81.28411553321183</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>6607.107438016528</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ma: 1, 1</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>564</v>
+        <v>640</v>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -3738,35 +3738,35 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>22.57142857142857</v>
+        <v>31.44444444444444</v>
       </c>
       <c r="G11" t="n">
-        <v>9.240549502169273</v>
+        <v>47.13953545028988</v>
       </c>
       <c r="H11" t="n">
-        <v>85.38775510204081</v>
+        <v>2222.135802469136</v>
       </c>
       <c r="I11" t="n">
-        <v>19</v>
+        <v>76.77777777777777</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>75.89726649707745</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>5760.395061728395</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 1</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>868</v>
+        <v>564</v>
       </c>
       <c r="C12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -3775,22 +3775,22 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>39.94594594594594</v>
+        <v>22.57142857142857</v>
       </c>
       <c r="G12" t="n">
-        <v>32.38780713682563</v>
+        <v>9.240549502169273</v>
       </c>
       <c r="H12" t="n">
-        <v>1048.970051132213</v>
+        <v>85.38775510204081</v>
       </c>
       <c r="I12" t="n">
-        <v>98.76470588235294</v>
+        <v>19</v>
       </c>
       <c r="J12" t="n">
-        <v>61.01738364815748</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>3723.121107266436</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug behoben; analyse topology hinzugefügt
</commit_message>
<xml_diff>
--- a/analysis_solution/machine_statistics/Machine_data.xlsx
+++ b/analysis_solution/machine_statistics/Machine_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,16 +499,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.2</t>
+          <t>ProductGroup.EIGHT.4</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="D2" t="n">
         <v>8</v>
@@ -520,37 +520,37 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1024</v>
       </c>
       <c r="J2" t="n">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.3</t>
+          <t>ProductGroup.FOUR.4</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
@@ -562,16 +562,16 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H3" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I3" t="n">
-        <v>324</v>
+        <v>144</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>181</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -583,16 +583,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.3</t>
+          <t>ProductGroup.TWO.4</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
@@ -604,16 +604,16 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="H4" t="n">
-        <v>27</v>
+        <v>29.97776954122282</v>
       </c>
       <c r="I4" t="n">
-        <v>729</v>
+        <v>898.6666666666666</v>
       </c>
       <c r="J4" t="n">
-        <v>239</v>
+        <v>115</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -625,19 +625,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 1, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.1</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>564</v>
+        <v>356</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -646,40 +646,40 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="H5" t="n">
-        <v>9.856107606091623</v>
+        <v>22.05296654269745</v>
       </c>
       <c r="I5" t="n">
-        <v>97.14285714285714</v>
+        <v>486.3333333333333</v>
       </c>
       <c r="J5" t="n">
-        <v>272.1666666666667</v>
+        <v>46.5</v>
       </c>
       <c r="K5" t="n">
-        <v>584.0149589027856</v>
+        <v>0.8660254037844386</v>
       </c>
       <c r="L5" t="n">
-        <v>341073.4722222222</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.1</t>
+          <t>ProductGroup.TWELVE.4</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -688,16 +688,16 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="H6" t="n">
-        <v>16</v>
+        <v>26.8824602048746</v>
       </c>
       <c r="I6" t="n">
-        <v>256</v>
+        <v>722.6666666666666</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>315</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -709,19 +709,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.3</t>
+          <t>ProductGroup.ONE.4</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>564</v>
+        <v>32</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -730,16 +730,16 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>27.2</v>
+        <v>32</v>
       </c>
       <c r="H7" t="n">
-        <v>13.6</v>
+        <v>32</v>
       </c>
       <c r="I7" t="n">
-        <v>184.96</v>
+        <v>1024</v>
       </c>
       <c r="J7" t="n">
-        <v>497</v>
+        <v>89</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -751,19 +751,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.3</t>
+          <t>ProductGroup.THIRTEEN.4</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -772,40 +772,40 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>14</v>
+        <v>21.5</v>
       </c>
       <c r="H8" t="n">
-        <v>14</v>
+        <v>25.35251466817444</v>
       </c>
       <c r="I8" t="n">
-        <v>196</v>
+        <v>642.75</v>
       </c>
       <c r="J8" t="n">
-        <v>1689</v>
+        <v>348</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>259</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>67081</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.1</t>
+          <t>ProductGroup.FIFTEEN.4</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -814,16 +814,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -835,19 +835,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 0, 1</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.4</t>
+          <t>ProductGroup.FOURTEEN.4</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -859,34 +859,34 @@
         <v>30</v>
       </c>
       <c r="H10" t="n">
-        <v>30</v>
+        <v>30.13303834663873</v>
       </c>
       <c r="I10" t="n">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="J10" t="n">
-        <v>43</v>
+        <v>320</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>233</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>54289</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.1</t>
+          <t>ProductGroup.NINE.4</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D11" t="n">
         <v>8</v>
@@ -898,33 +898,33 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>18</v>
+        <v>30.5</v>
       </c>
       <c r="H11" t="n">
-        <v>18</v>
+        <v>30.5736814924209</v>
       </c>
       <c r="I11" t="n">
-        <v>324</v>
+        <v>934.75</v>
       </c>
       <c r="J11" t="n">
-        <v>527</v>
+        <v>85.5</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.2</t>
+          <t>ProductGroup.TEN.4</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -940,16 +940,16 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="H12" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I12" t="n">
-        <v>225</v>
+        <v>1296</v>
       </c>
       <c r="J12" t="n">
-        <v>1352</v>
+        <v>88</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
@@ -961,12 +961,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.3</t>
+          <t>ProductGroup.THREE.4</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -982,16 +982,16 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H13" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I13" t="n">
-        <v>64</v>
+        <v>196</v>
       </c>
       <c r="J13" t="n">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1003,16 +1003,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.3</t>
+          <t>ProductGroup.ELEVEN.4</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D14" t="n">
         <v>8</v>
@@ -1024,16 +1024,16 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H14" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I14" t="n">
-        <v>324</v>
+        <v>1024</v>
       </c>
       <c r="J14" t="n">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1045,16 +1045,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.2</t>
+          <t>ProductGroup.TWELVE.3</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>180</v>
+        <v>64</v>
       </c>
       <c r="D15" t="n">
         <v>8</v>
@@ -1066,16 +1066,16 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H15" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I15" t="n">
-        <v>324</v>
+        <v>256</v>
       </c>
       <c r="J15" t="n">
-        <v>1703</v>
+        <v>163</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1087,58 +1087,58 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.4</t>
+          <t>ProductGroup.THREE.1</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="D16" t="n">
-        <v>7.846153846153846</v>
+        <v>8</v>
       </c>
       <c r="E16" t="n">
-        <v>0.532938710021193</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2840236686390533</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>62</v>
+        <v>31.5</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>36.83408747342602</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1356.75</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>587</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>93025</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.4</t>
+          <t>ProductGroup.SEVEN.3</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>180</v>
+        <v>356</v>
       </c>
       <c r="D17" t="n">
         <v>8</v>
@@ -1150,22 +1150,22 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>42.85714285714285</v>
+        <v>42.5</v>
       </c>
       <c r="H17" t="n">
-        <v>19.7370469019092</v>
+        <v>19.48717526990508</v>
       </c>
       <c r="I17" t="n">
-        <v>389.5510204081633</v>
+        <v>379.75</v>
       </c>
       <c r="J17" t="n">
-        <v>27.5</v>
+        <v>31.5</v>
       </c>
       <c r="K17" t="n">
-        <v>14.5</v>
+        <v>9.5</v>
       </c>
       <c r="L17" t="n">
-        <v>210.25</v>
+        <v>90.25</v>
       </c>
     </row>
     <row r="18">
@@ -1176,11 +1176,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.1</t>
+          <t>ProductGroup.FOUR.1</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D18" t="n">
         <v>8</v>
@@ -1192,22 +1192,22 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H18" t="n">
-        <v>16</v>
+        <v>29.8496231131986</v>
       </c>
       <c r="I18" t="n">
-        <v>256</v>
+        <v>891</v>
       </c>
       <c r="J18" t="n">
-        <v>926</v>
+        <v>24</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.3</t>
+          <t>ProductGroup.ELEVEN.1</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>180</v>
+        <v>28</v>
       </c>
       <c r="D19" t="n">
         <v>8</v>
@@ -1234,16 +1234,16 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>38.66666666666666</v>
+        <v>33</v>
       </c>
       <c r="H19" t="n">
-        <v>27.77688887466621</v>
+        <v>33</v>
       </c>
       <c r="I19" t="n">
-        <v>771.5555555555555</v>
+        <v>1089</v>
       </c>
       <c r="J19" t="n">
-        <v>444</v>
+        <v>63</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -1260,11 +1260,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.1</t>
+          <t>ProductGroup.ONE.2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D20" t="n">
         <v>8</v>
@@ -1276,22 +1276,22 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="H20" t="n">
-        <v>17</v>
+        <v>37.00450423034111</v>
       </c>
       <c r="I20" t="n">
-        <v>289</v>
+        <v>1369.333333333333</v>
       </c>
       <c r="J20" t="n">
-        <v>133</v>
+        <v>31.5</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>42.25</v>
       </c>
     </row>
     <row r="21">
@@ -1306,7 +1306,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="D21" t="n">
         <v>8</v>
@@ -1318,22 +1318,22 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="H21" t="n">
-        <v>1.632993161855452</v>
+        <v>23.2163735324878</v>
       </c>
       <c r="I21" t="n">
-        <v>2.666666666666667</v>
+        <v>539</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>52.5</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>756.25</v>
       </c>
     </row>
     <row r="22">
@@ -1344,11 +1344,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.1</t>
+          <t>ProductGroup.TWO.3</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D22" t="n">
         <v>8</v>
@@ -1360,79 +1360,79 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>17</v>
+        <v>43.5</v>
       </c>
       <c r="H22" t="n">
-        <v>17</v>
+        <v>26.7348087705897</v>
       </c>
       <c r="I22" t="n">
-        <v>289</v>
+        <v>714.75</v>
       </c>
       <c r="J22" t="n">
-        <v>25</v>
+        <v>354.5</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>59.5</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>3540.25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.4</t>
+          <t>ProductGroup.TEN.1</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>8</v>
+        <v>131</v>
       </c>
       <c r="D23" t="n">
-        <v>8</v>
+        <v>7.969465648854962</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>0.3481451679692024</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.1212050579803042</v>
       </c>
       <c r="G23" t="n">
-        <v>12</v>
+        <v>23.2</v>
       </c>
       <c r="H23" t="n">
-        <v>12</v>
+        <v>19.62039754948916</v>
       </c>
       <c r="I23" t="n">
-        <v>144</v>
+        <v>384.96</v>
       </c>
       <c r="J23" t="n">
-        <v>591</v>
+        <v>87.5</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>45.5</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>2070.25</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.4</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>8</v>
+        <v>564</v>
       </c>
       <c r="D24" t="n">
         <v>8</v>
@@ -1444,37 +1444,37 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>15</v>
+        <v>57.81818181818182</v>
       </c>
       <c r="H24" t="n">
-        <v>15</v>
+        <v>19.49274075518269</v>
       </c>
       <c r="I24" t="n">
-        <v>225</v>
+        <v>379.9669421487604</v>
       </c>
       <c r="J24" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>1.632993161855452</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.4</t>
+          <t>ProductGroup.FOUR.2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D25" t="n">
         <v>8</v>
@@ -1486,79 +1486,79 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H25" t="n">
-        <v>12</v>
+        <v>18.49324200890693</v>
       </c>
       <c r="I25" t="n">
-        <v>144</v>
+        <v>342</v>
       </c>
       <c r="J25" t="n">
-        <v>181</v>
+        <v>700</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>668</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>446224</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.4</t>
+          <t>ProductGroup.EIGHT.3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D26" t="n">
-        <v>7.666666666666667</v>
+        <v>8</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4714045207910317</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.2222222222222222</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>31.51190251317746</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>993</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.4</t>
+          <t>ProductGroup.FIFTEEN.3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="D27" t="n">
         <v>8</v>
@@ -1570,37 +1570,37 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="H27" t="n">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="I27" t="n">
-        <v>1444</v>
+        <v>324</v>
       </c>
       <c r="J27" t="n">
-        <v>94</v>
+        <v>35.5</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>42.25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.4</t>
+          <t>ProductGroup.THREE.3</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>564</v>
+        <v>120</v>
       </c>
       <c r="D28" t="n">
         <v>8</v>
@@ -1612,37 +1612,37 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>56.83333333333334</v>
+        <v>37.5</v>
       </c>
       <c r="H28" t="n">
-        <v>17.82242657128621</v>
+        <v>37.55995207664674</v>
       </c>
       <c r="I28" t="n">
-        <v>317.6388888888889</v>
+        <v>1410.75</v>
       </c>
       <c r="J28" t="n">
-        <v>46.33333333333334</v>
+        <v>34.5</v>
       </c>
       <c r="K28" t="n">
-        <v>1.795054935711502</v>
+        <v>6.5</v>
       </c>
       <c r="L28" t="n">
-        <v>3.222222222222223</v>
+        <v>42.25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.3</t>
+          <t>ProductGroup.ONE.3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D29" t="n">
         <v>8</v>
@@ -1654,37 +1654,37 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>26</v>
+        <v>61.5</v>
       </c>
       <c r="H29" t="n">
-        <v>26</v>
+        <v>57.19047123428867</v>
       </c>
       <c r="I29" t="n">
-        <v>676</v>
+        <v>3270.75</v>
       </c>
       <c r="J29" t="n">
-        <v>23</v>
+        <v>28.5</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>210.25</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.3</t>
+          <t>ProductGroup.TWO.2</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="D30" t="n">
         <v>8</v>
@@ -1696,64 +1696,1240 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>24.16609194718914</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>584</v>
       </c>
       <c r="J30" t="n">
-        <v>167</v>
+        <v>1014.5</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>715.5</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>511940.25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ProductGroup.THIRTEEN.1</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>20</v>
+      </c>
+      <c r="D31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>41</v>
+      </c>
+      <c r="H31" t="n">
+        <v>52.3354564325181</v>
+      </c>
+      <c r="I31" t="n">
+        <v>2739</v>
+      </c>
+      <c r="J31" t="n">
+        <v>346.5</v>
+      </c>
+      <c r="K31" t="n">
+        <v>218.5</v>
+      </c>
+      <c r="L31" t="n">
+        <v>47742.25</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ProductGroup.ELEVEN.3</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>52</v>
+      </c>
+      <c r="D32" t="n">
+        <v>8</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>54.66666666666666</v>
+      </c>
+      <c r="H32" t="n">
+        <v>58.11100488624241</v>
+      </c>
+      <c r="I32" t="n">
+        <v>3376.888888888889</v>
+      </c>
+      <c r="J32" t="n">
+        <v>29</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOURTEEN.1</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>51</v>
+      </c>
+      <c r="D33" t="n">
+        <v>7.941176470588236</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.4159451654038515</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.1730103806228374</v>
+      </c>
+      <c r="G33" t="n">
+        <v>24</v>
+      </c>
+      <c r="H33" t="n">
+        <v>16.97056274847714</v>
+      </c>
+      <c r="I33" t="n">
+        <v>288</v>
+      </c>
+      <c r="J33" t="n">
+        <v>444</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Ma: 0, 1</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ProductGroup.TWELVE.4</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>92</v>
+      </c>
+      <c r="D34" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>30</v>
+      </c>
+      <c r="H34" t="n">
+        <v>30</v>
+      </c>
+      <c r="I34" t="n">
+        <v>900</v>
+      </c>
+      <c r="J34" t="n">
+        <v>43</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Ma: 3, 1</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOURTEEN.1</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>40</v>
+      </c>
+      <c r="D35" t="n">
+        <v>10</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>55</v>
+      </c>
+      <c r="H35" t="n">
+        <v>55</v>
+      </c>
+      <c r="I35" t="n">
+        <v>3025</v>
+      </c>
+      <c r="J35" t="n">
+        <v>24</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>Ma: 1, 2</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOUR.3</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>52</v>
+      </c>
+      <c r="D36" t="n">
+        <v>8</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>34</v>
+      </c>
+      <c r="H36" t="n">
+        <v>34</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1156</v>
+      </c>
+      <c r="J36" t="n">
+        <v>23</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ProductGroup.SEVEN.1</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>356</v>
+      </c>
+      <c r="D37" t="n">
+        <v>8</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>42</v>
+      </c>
+      <c r="H37" t="n">
+        <v>25.79922479455536</v>
+      </c>
+      <c r="I37" t="n">
+        <v>665.6</v>
+      </c>
+      <c r="J37" t="n">
+        <v>36</v>
+      </c>
+      <c r="K37" t="n">
+        <v>11.7756811551038</v>
+      </c>
+      <c r="L37" t="n">
+        <v>138.6666666666667</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>ProductGroup.TWO.1</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C38" t="n">
+        <v>210</v>
+      </c>
+      <c r="D38" t="n">
+        <v>8</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="H38" t="n">
+        <v>26.32014437650371</v>
+      </c>
+      <c r="I38" t="n">
+        <v>692.75</v>
+      </c>
+      <c r="J38" t="n">
+        <v>477</v>
+      </c>
+      <c r="K38" t="n">
+        <v>455</v>
+      </c>
+      <c r="L38" t="n">
+        <v>207025</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Ma: 1, 2</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ProductGroup.THIRTEEN.3</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>8</v>
+      </c>
+      <c r="D39" t="n">
+        <v>8</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>167</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Ma: 2, 1</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ProductGroup.TWELVE.3</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>92</v>
+      </c>
+      <c r="D40" t="n">
+        <v>10</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>14</v>
+      </c>
+      <c r="H40" t="n">
+        <v>14</v>
+      </c>
+      <c r="I40" t="n">
+        <v>196</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1771</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Ma: 2, 1</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ProductGroup.ELEVEN.1</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>24</v>
+      </c>
+      <c r="D41" t="n">
+        <v>10</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>44</v>
+      </c>
+      <c r="H41" t="n">
+        <v>44</v>
+      </c>
+      <c r="I41" t="n">
+        <v>1936</v>
+      </c>
+      <c r="J41" t="n">
+        <v>21</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Ma: 2, 1</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ProductGroup.SEVEN.3</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>564</v>
+      </c>
+      <c r="D42" t="n">
+        <v>10</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>17</v>
+      </c>
+      <c r="H42" t="n">
+        <v>17</v>
+      </c>
+      <c r="I42" t="n">
+        <v>289</v>
+      </c>
+      <c r="J42" t="n">
+        <v>33</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Ma: 0, 2</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ProductGroup.TWO.4</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
         <v>180</v>
       </c>
-      <c r="D31" t="n">
-        <v>8</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="n">
-        <v>22</v>
-      </c>
-      <c r="H31" t="n">
-        <v>15.57776192739723</v>
-      </c>
-      <c r="I31" t="n">
-        <v>242.6666666666667</v>
-      </c>
-      <c r="J31" t="n">
-        <v>472.5</v>
-      </c>
-      <c r="K31" t="n">
-        <v>450.5</v>
-      </c>
-      <c r="L31" t="n">
-        <v>202950.25</v>
+      <c r="D43" t="n">
+        <v>8</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>47.33333333333334</v>
+      </c>
+      <c r="H43" t="n">
+        <v>21.31248981752771</v>
+      </c>
+      <c r="I43" t="n">
+        <v>454.2222222222222</v>
+      </c>
+      <c r="J43" t="n">
+        <v>44</v>
+      </c>
+      <c r="K43" t="n">
+        <v>2</v>
+      </c>
+      <c r="L43" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Ma: 0, 2</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOUR.4</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>16</v>
+      </c>
+      <c r="D44" t="n">
+        <v>8</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>29</v>
+      </c>
+      <c r="H44" t="n">
+        <v>29</v>
+      </c>
+      <c r="I44" t="n">
+        <v>841</v>
+      </c>
+      <c r="J44" t="n">
+        <v>44</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Ma: 0, 2</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ProductGroup.FIFTEEN.4</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>4</v>
+      </c>
+      <c r="D45" t="n">
+        <v>8</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>21</v>
+      </c>
+      <c r="H45" t="n">
+        <v>21</v>
+      </c>
+      <c r="I45" t="n">
+        <v>441</v>
+      </c>
+      <c r="J45" t="n">
+        <v>37</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Ma: 0, 2</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ProductGroup.ONE.4</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>16</v>
+      </c>
+      <c r="D46" t="n">
+        <v>8</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>85.33333333333333</v>
+      </c>
+      <c r="H46" t="n">
+        <v>77.72315542287825</v>
+      </c>
+      <c r="I46" t="n">
+        <v>6040.888888888888</v>
+      </c>
+      <c r="J46" t="n">
+        <v>88</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Ma: 0, 2</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ProductGroup.TEN.4</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>44</v>
+      </c>
+      <c r="D47" t="n">
+        <v>8</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>39.33333333333334</v>
+      </c>
+      <c r="H47" t="n">
+        <v>27.82484900627894</v>
+      </c>
+      <c r="I47" t="n">
+        <v>774.2222222222223</v>
+      </c>
+      <c r="J47" t="n">
+        <v>73</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Ma: 0, 2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ProductGroup.THREE.4</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>36</v>
+      </c>
+      <c r="D48" t="n">
+        <v>8</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>57.6</v>
+      </c>
+      <c r="H48" t="n">
+        <v>47.58823383988946</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2264.64</v>
+      </c>
+      <c r="J48" t="n">
+        <v>85</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Ma: 0, 2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ProductGroup.ELEVEN.4</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>28</v>
+      </c>
+      <c r="D49" t="n">
+        <v>8</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>33</v>
+      </c>
+      <c r="H49" t="n">
+        <v>33</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1089</v>
+      </c>
+      <c r="J49" t="n">
+        <v>82</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ProductGroup.THREE.2</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>120</v>
+      </c>
+      <c r="D50" t="n">
+        <v>8</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>27.33333333333333</v>
+      </c>
+      <c r="H50" t="n">
+        <v>38.6551707048646</v>
+      </c>
+      <c r="I50" t="n">
+        <v>1494.222222222222</v>
+      </c>
+      <c r="J50" t="n">
+        <v>241.5</v>
+      </c>
+      <c r="K50" t="n">
+        <v>237.5</v>
+      </c>
+      <c r="L50" t="n">
+        <v>56406.25</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ProductGroup.TWO.1</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>76</v>
+      </c>
+      <c r="D51" t="n">
+        <v>8</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>32</v>
+      </c>
+      <c r="H51" t="n">
+        <v>32</v>
+      </c>
+      <c r="I51" t="n">
+        <v>1024</v>
+      </c>
+      <c r="J51" t="n">
+        <v>177</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ProductGroup.NINE.3</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>104</v>
+      </c>
+      <c r="D52" t="n">
+        <v>8</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>18</v>
+      </c>
+      <c r="H52" t="n">
+        <v>18</v>
+      </c>
+      <c r="I52" t="n">
+        <v>324</v>
+      </c>
+      <c r="J52" t="n">
+        <v>85.5</v>
+      </c>
+      <c r="K52" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="L52" t="n">
+        <v>1560.25</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOUR.3</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>16</v>
+      </c>
+      <c r="D53" t="n">
+        <v>8</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>50</v>
+      </c>
+      <c r="H53" t="n">
+        <v>42.55192905928786</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1810.666666666667</v>
+      </c>
+      <c r="J53" t="n">
+        <v>29</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ProductGroup.ONE.1</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>48</v>
+      </c>
+      <c r="D54" t="n">
+        <v>8</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="H54" t="n">
+        <v>20.80264406271472</v>
+      </c>
+      <c r="I54" t="n">
+        <v>432.75</v>
+      </c>
+      <c r="J54" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K54" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L54" t="n">
+        <v>72.25</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ProductGroup.THIRTEEN.3</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>12</v>
+      </c>
+      <c r="D55" t="n">
+        <v>8</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>65</v>
+      </c>
+      <c r="H55" t="n">
+        <v>65</v>
+      </c>
+      <c r="I55" t="n">
+        <v>4225</v>
+      </c>
+      <c r="J55" t="n">
+        <v>224</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ProductGroup.SEVEN.1</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>30</v>
+      </c>
+      <c r="D56" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.077032961426901</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="G56" t="n">
+        <v>68</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>ProductGroup.TEN.3</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>96</v>
+      </c>
+      <c r="D57" t="n">
+        <v>8</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>33.66666666666666</v>
+      </c>
+      <c r="H57" t="n">
+        <v>25.70127536826831</v>
+      </c>
+      <c r="I57" t="n">
+        <v>660.5555555555555</v>
+      </c>
+      <c r="J57" t="n">
+        <v>223</v>
+      </c>
+      <c r="K57" t="n">
+        <v>175</v>
+      </c>
+      <c r="L57" t="n">
+        <v>30625</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Ma: 1, 3</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ProductGroup.EIGHT.1</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>36</v>
+      </c>
+      <c r="D58" t="n">
+        <v>8</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>19</v>
+      </c>
+      <c r="H58" t="n">
+        <v>19.05255888325765</v>
+      </c>
+      <c r="I58" t="n">
+        <v>363</v>
+      </c>
+      <c r="J58" t="n">
+        <v>97</v>
+      </c>
+      <c r="K58" t="n">
+        <v>65</v>
+      </c>
+      <c r="L58" t="n">
+        <v>4225</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Ma: 1, 1</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ProductGroup.SEVEN.1</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>564</v>
+      </c>
+      <c r="D59" t="n">
+        <v>10</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>26.57142857142857</v>
+      </c>
+      <c r="H59" t="n">
+        <v>13.92692297937593</v>
+      </c>
+      <c r="I59" t="n">
+        <v>193.9591836734694</v>
+      </c>
+      <c r="J59" t="n">
+        <v>101.3</v>
+      </c>
+      <c r="K59" t="n">
+        <v>263.3904136448402</v>
+      </c>
+      <c r="L59" t="n">
+        <v>69374.51000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1835,11 +3011,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>180</v>
+        <v>964</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -1851,72 +3027,72 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>18</v>
+        <v>31.8</v>
       </c>
       <c r="G2" t="n">
-        <v>22.76839915321233</v>
+        <v>29.28412539243746</v>
       </c>
       <c r="H2" t="n">
-        <v>518.4</v>
+        <v>857.5600000000004</v>
       </c>
       <c r="I2" t="n">
-        <v>95</v>
+        <v>142.25</v>
       </c>
       <c r="J2" t="n">
-        <v>103.2569610244268</v>
+        <v>157.7351815544015</v>
       </c>
       <c r="K2" t="n">
-        <v>10662</v>
+        <v>24880.3875</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ma: 1, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>564</v>
+        <v>1127</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>7.996450754214729</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.1190982199507543</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.01418438599543826</v>
       </c>
       <c r="F3" t="n">
-        <v>24</v>
+        <v>34.23255813953488</v>
       </c>
       <c r="G3" t="n">
-        <v>9.856107606091623</v>
+        <v>29.15303423460119</v>
       </c>
       <c r="H3" t="n">
-        <v>97.14285714285714</v>
+        <v>849.8994050838287</v>
       </c>
       <c r="I3" t="n">
-        <v>272.1666666666667</v>
+        <v>160.1875</v>
       </c>
       <c r="J3" t="n">
-        <v>584.0149589027856</v>
+        <v>221.5643864517716</v>
       </c>
       <c r="K3" t="n">
-        <v>341073.4722222222</v>
+        <v>49090.77734375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40</v>
+        <v>564</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1925,59 +3101,59 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>16</v>
+        <v>57.81818181818182</v>
       </c>
       <c r="G4" t="n">
-        <v>16</v>
+        <v>19.49274075518269</v>
       </c>
       <c r="H4" t="n">
-        <v>256</v>
+        <v>379.9669421487604</v>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1.632993161855452</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>656</v>
+        <v>663</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>7.995475113122172</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.1164224464277702</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.01355418603222702</v>
       </c>
       <c r="F5" t="n">
-        <v>23</v>
+        <v>38.29268292682926</v>
       </c>
       <c r="G5" t="n">
-        <v>14.0356688476182</v>
+        <v>45.19564186978005</v>
       </c>
       <c r="H5" t="n">
-        <v>197</v>
+        <v>2042.646044021416</v>
       </c>
       <c r="I5" t="n">
-        <v>1093</v>
+        <v>288.0588235294118</v>
       </c>
       <c r="J5" t="n">
-        <v>596</v>
+        <v>490.4157264761057</v>
       </c>
       <c r="K5" t="n">
-        <v>355216</v>
+        <v>240507.5847750866</v>
       </c>
     </row>
     <row r="6">
@@ -2020,14 +3196,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>332</v>
+        <v>40</v>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -2036,72 +3212,72 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>15.4</v>
+        <v>55</v>
       </c>
       <c r="G7" t="n">
-        <v>16.34747686953556</v>
+        <v>55</v>
       </c>
       <c r="H7" t="n">
-        <v>267.24</v>
+        <v>3025</v>
       </c>
       <c r="I7" t="n">
-        <v>728</v>
+        <v>24</v>
       </c>
       <c r="J7" t="n">
-        <v>686.6740129056873</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>471521.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>193</v>
+        <v>626</v>
       </c>
       <c r="C8" t="n">
-        <v>7.989637305699482</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1435897042544151</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02061800316787041</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>45.25</v>
+        <v>36.33333333333334</v>
       </c>
       <c r="G8" t="n">
-        <v>19.51762024428183</v>
+        <v>28.78464096624371</v>
       </c>
       <c r="H8" t="n">
-        <v>380.9375</v>
+        <v>828.5555555555555</v>
       </c>
       <c r="I8" t="n">
-        <v>27.5</v>
+        <v>178.8571428571429</v>
       </c>
       <c r="J8" t="n">
-        <v>14.5</v>
+        <v>311.1960468769433</v>
       </c>
       <c r="K8" t="n">
-        <v>210.25</v>
+        <v>96842.97959183672</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>393</v>
+        <v>680</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2110,109 +3286,109 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G9" t="n">
-        <v>22.83272505272495</v>
+        <v>31.44837038703277</v>
       </c>
       <c r="H9" t="n">
-        <v>521.3333333333334</v>
+        <v>989</v>
       </c>
       <c r="I9" t="n">
-        <v>382</v>
+        <v>608.3333333333334</v>
       </c>
       <c r="J9" t="n">
-        <v>349.7248918793171</v>
+        <v>822.1440803708854</v>
       </c>
       <c r="K9" t="n">
-        <v>122307.5</v>
+        <v>675920.8888888889</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>155</v>
+        <v>324</v>
       </c>
       <c r="C10" t="n">
-        <v>7.993548387096774</v>
+        <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>0.08006241061929596</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.006409989594172755</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>24.22222222222222</v>
+        <v>48.34782608695652</v>
       </c>
       <c r="G10" t="n">
-        <v>27.16933638324964</v>
+        <v>45.07636872035315</v>
       </c>
       <c r="H10" t="n">
-        <v>738.1728395061729</v>
+        <v>2031.879017013232</v>
       </c>
       <c r="I10" t="n">
-        <v>228.75</v>
+        <v>62.125</v>
       </c>
       <c r="J10" t="n">
-        <v>214.4602235847011</v>
+        <v>20.40488605702075</v>
       </c>
       <c r="K10" t="n">
-        <v>45993.1875</v>
+        <v>416.359375</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 1, 3</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>564</v>
+        <v>538</v>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>7.988847583643123</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.2584378489127825</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.0667901217506662</v>
       </c>
       <c r="F11" t="n">
-        <v>56.83333333333334</v>
+        <v>31.93103448275862</v>
       </c>
       <c r="G11" t="n">
-        <v>17.82242657128621</v>
+        <v>34.92448112268049</v>
       </c>
       <c r="H11" t="n">
-        <v>317.6388888888889</v>
+        <v>1219.719381688466</v>
       </c>
       <c r="I11" t="n">
-        <v>46.33333333333334</v>
+        <v>138.3846153846154</v>
       </c>
       <c r="J11" t="n">
-        <v>1.795054935711502</v>
+        <v>144.5212459555493</v>
       </c>
       <c r="K11" t="n">
-        <v>3.222222222222223</v>
+        <v>20886.39053254438</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 1, 1</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>240</v>
+        <v>564</v>
       </c>
       <c r="C12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -2221,22 +3397,22 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>19.66666666666667</v>
+        <v>26.57142857142857</v>
       </c>
       <c r="G12" t="n">
-        <v>20.66935466390333</v>
+        <v>13.92692297937593</v>
       </c>
       <c r="H12" t="n">
-        <v>427.2222222222222</v>
+        <v>193.9591836734694</v>
       </c>
       <c r="I12" t="n">
-        <v>283.75</v>
+        <v>101.3</v>
       </c>
       <c r="J12" t="n">
-        <v>373.7561872397566</v>
+        <v>263.3904136448402</v>
       </c>
       <c r="K12" t="n">
-        <v>139693.6875</v>
+        <v>69374.51000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QAP eingeführt und machine topologie wird angepasst
</commit_message>
<xml_diff>
--- a/analysis_solution/machine_statistics/Machine_data.xlsx
+++ b/analysis_solution/machine_statistics/Machine_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,19 +499,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.4</t>
+          <t>ProductGroup.EIGHT.1</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -520,40 +520,40 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H2" t="n">
-        <v>32</v>
+        <v>24.1039415863879</v>
       </c>
       <c r="I2" t="n">
-        <v>1024</v>
+        <v>581</v>
       </c>
       <c r="J2" t="n">
-        <v>69</v>
+        <v>30.66666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>20</v>
+        <v>5.90668171555645</v>
       </c>
       <c r="L2" t="n">
-        <v>400</v>
+        <v>34.88888888888889</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.4</t>
+          <t>ProductGroup.TEN.3</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -562,40 +562,40 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>12</v>
+        <v>29.71428571428572</v>
       </c>
       <c r="H3" t="n">
-        <v>12</v>
+        <v>27.86556649196939</v>
       </c>
       <c r="I3" t="n">
-        <v>144</v>
+        <v>776.4897959183673</v>
       </c>
       <c r="J3" t="n">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>139.3006341215526</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>19404.66666666667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.4</t>
+          <t>ProductGroup.ONE.1</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -604,40 +604,40 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>42</v>
+        <v>27.5</v>
       </c>
       <c r="H4" t="n">
-        <v>29.97776954122282</v>
+        <v>29.47456530637899</v>
       </c>
       <c r="I4" t="n">
-        <v>898.6666666666666</v>
+        <v>868.75</v>
       </c>
       <c r="J4" t="n">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.4</t>
+          <t>ProductGroup.THIRTEEN.3</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>356</v>
+        <v>32</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -646,40 +646,40 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>49</v>
+        <v>25.66666666666667</v>
       </c>
       <c r="H5" t="n">
-        <v>22.05296654269745</v>
+        <v>26.24034213869087</v>
       </c>
       <c r="I5" t="n">
-        <v>486.3333333333333</v>
+        <v>688.5555555555557</v>
       </c>
       <c r="J5" t="n">
-        <v>46.5</v>
+        <v>38</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8660254037844386</v>
+        <v>1.632993161855452</v>
       </c>
       <c r="L5" t="n">
-        <v>0.75</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.4</t>
+          <t>ProductGroup.SIX.3</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -688,16 +688,16 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="H6" t="n">
-        <v>26.8824602048746</v>
+        <v>22</v>
       </c>
       <c r="I6" t="n">
-        <v>722.6666666666666</v>
+        <v>484</v>
       </c>
       <c r="J6" t="n">
-        <v>315</v>
+        <v>41</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -709,19 +709,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.4</t>
+          <t>ProductGroup.SEVEN.1</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>32</v>
+        <v>696</v>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -730,16 +730,16 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>32</v>
+        <v>33.6</v>
       </c>
       <c r="H7" t="n">
-        <v>32</v>
+        <v>22.21350940306371</v>
       </c>
       <c r="I7" t="n">
-        <v>1024</v>
+        <v>493.4399999999999</v>
       </c>
       <c r="J7" t="n">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -751,19 +751,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.4</t>
+          <t>ProductGroup.FOUR.3</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -772,40 +772,40 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>21.5</v>
+        <v>46.44444444444444</v>
       </c>
       <c r="H8" t="n">
-        <v>25.35251466817444</v>
+        <v>42.64351223577238</v>
       </c>
       <c r="I8" t="n">
-        <v>642.75</v>
+        <v>1818.469135802469</v>
       </c>
       <c r="J8" t="n">
-        <v>348</v>
+        <v>34.33333333333334</v>
       </c>
       <c r="K8" t="n">
-        <v>259</v>
+        <v>6.649979114420002</v>
       </c>
       <c r="L8" t="n">
-        <v>67081</v>
+        <v>44.22222222222223</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.4</t>
+          <t>ProductGroup.TWO.1</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>352</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -814,40 +814,40 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>15</v>
+        <v>27.14285714285714</v>
       </c>
       <c r="H9" t="n">
-        <v>15</v>
+        <v>26.40037105490631</v>
       </c>
       <c r="I9" t="n">
-        <v>225</v>
+        <v>696.9795918367347</v>
       </c>
       <c r="J9" t="n">
-        <v>49</v>
+        <v>1483.333333333333</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>2040.474835805518</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>4163537.555555556</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.4</t>
+          <t>ProductGroup.NINE.3</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>56</v>
+        <v>152</v>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -856,40 +856,40 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>30</v>
+        <v>27.33333333333333</v>
       </c>
       <c r="H10" t="n">
-        <v>30.13303834663873</v>
+        <v>35.5089972948954</v>
       </c>
       <c r="I10" t="n">
-        <v>908</v>
+        <v>1260.888888888889</v>
       </c>
       <c r="J10" t="n">
-        <v>320</v>
+        <v>106</v>
       </c>
       <c r="K10" t="n">
-        <v>233</v>
+        <v>94.04608799235972</v>
       </c>
       <c r="L10" t="n">
-        <v>54289</v>
+        <v>8844.666666666666</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.4</t>
+          <t>ProductGroup.THREE.2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="D11" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -898,40 +898,40 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>30.5</v>
+        <v>24</v>
       </c>
       <c r="H11" t="n">
-        <v>30.5736814924209</v>
+        <v>25.79405616287081</v>
       </c>
       <c r="I11" t="n">
-        <v>934.75</v>
+        <v>665.3333333333334</v>
       </c>
       <c r="J11" t="n">
-        <v>85.5</v>
+        <v>298</v>
       </c>
       <c r="K11" t="n">
-        <v>3.5</v>
+        <v>294.2425303498233</v>
       </c>
       <c r="L11" t="n">
-        <v>12.25</v>
+        <v>86578.66666666667</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.4</t>
+          <t>ProductGroup.SEVEN.1</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>52</v>
+        <v>564</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -940,28 +940,28 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>36</v>
+        <v>25.42857142857143</v>
       </c>
       <c r="H12" t="n">
-        <v>36</v>
+        <v>12.86031706848788</v>
       </c>
       <c r="I12" t="n">
-        <v>1296</v>
+        <v>165.3877551020408</v>
       </c>
       <c r="J12" t="n">
-        <v>88</v>
+        <v>93.18181818181819</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>253.5448026328853</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>64284.96694214876</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -970,10 +970,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="D13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -982,40 +982,40 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>14</v>
+        <v>43.33333333333334</v>
       </c>
       <c r="H13" t="n">
-        <v>14</v>
+        <v>30.7607253201582</v>
       </c>
       <c r="I13" t="n">
-        <v>196</v>
+        <v>946.2222222222222</v>
       </c>
       <c r="J13" t="n">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>5929</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.4</t>
+          <t>ProductGroup.FOURTEEN.4</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D14" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1024,40 +1024,40 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>32</v>
+        <v>25.66666666666667</v>
       </c>
       <c r="H14" t="n">
-        <v>32</v>
+        <v>29.56161174376135</v>
       </c>
       <c r="I14" t="n">
-        <v>1024</v>
+        <v>873.8888888888887</v>
       </c>
       <c r="J14" t="n">
-        <v>88</v>
+        <v>76.33333333333333</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>0.9428090415820634</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.888888888888889</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.3</t>
+          <t>ProductGroup.ONE.4</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1066,16 +1066,16 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H15" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I15" t="n">
-        <v>256</v>
+        <v>784</v>
       </c>
       <c r="J15" t="n">
-        <v>163</v>
+        <v>77</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1087,19 +1087,19 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.1</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>120</v>
+        <v>356</v>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1108,40 +1108,40 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>31.5</v>
+        <v>46</v>
       </c>
       <c r="H16" t="n">
-        <v>36.83408747342602</v>
+        <v>20.591260281974</v>
       </c>
       <c r="I16" t="n">
-        <v>1356.75</v>
+        <v>424</v>
       </c>
       <c r="J16" t="n">
-        <v>587</v>
+        <v>54.5</v>
       </c>
       <c r="K16" t="n">
-        <v>305</v>
+        <v>16.393596310755</v>
       </c>
       <c r="L16" t="n">
-        <v>93025</v>
+        <v>268.75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.3</t>
+          <t>ProductGroup.NINE.4</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>356</v>
+        <v>92</v>
       </c>
       <c r="D17" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1150,40 +1150,40 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>42.5</v>
+        <v>30.5</v>
       </c>
       <c r="H17" t="n">
-        <v>19.48717526990508</v>
+        <v>30.70423423568808</v>
       </c>
       <c r="I17" t="n">
-        <v>379.75</v>
+        <v>942.75</v>
       </c>
       <c r="J17" t="n">
-        <v>31.5</v>
+        <v>77</v>
       </c>
       <c r="K17" t="n">
-        <v>9.5</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>90.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.1</t>
+          <t>ProductGroup.THIRTEEN.4</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="D18" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1192,40 +1192,40 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>27</v>
+        <v>30.66666666666667</v>
       </c>
       <c r="H18" t="n">
-        <v>29.8496231131986</v>
+        <v>30.78239034830719</v>
       </c>
       <c r="I18" t="n">
-        <v>891</v>
+        <v>947.5555555555555</v>
       </c>
       <c r="J18" t="n">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="K18" t="n">
-        <v>1</v>
+        <v>17.79513042005219</v>
       </c>
       <c r="L18" t="n">
-        <v>1</v>
+        <v>316.6666666666667</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.1</t>
+          <t>ProductGroup.FOUR.4</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D19" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1234,40 +1234,40 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>33</v>
+        <v>32.5</v>
       </c>
       <c r="H19" t="n">
-        <v>33</v>
+        <v>32.50769139757544</v>
       </c>
       <c r="I19" t="n">
-        <v>1089</v>
+        <v>1056.75</v>
       </c>
       <c r="J19" t="n">
-        <v>63</v>
+        <v>65.5</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>240.25</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.2</t>
+          <t>ProductGroup.FIFTEEN.4</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D20" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1276,40 +1276,40 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="H20" t="n">
-        <v>37.00450423034111</v>
+        <v>27.44084546802449</v>
       </c>
       <c r="I20" t="n">
-        <v>1369.333333333333</v>
+        <v>753</v>
       </c>
       <c r="J20" t="n">
-        <v>31.5</v>
+        <v>59</v>
       </c>
       <c r="K20" t="n">
-        <v>6.5</v>
+        <v>16</v>
       </c>
       <c r="L20" t="n">
-        <v>42.25</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.3</t>
+          <t>ProductGroup.EIGHT.4</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D21" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1318,40 +1318,40 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>21</v>
+        <v>34.33333333333334</v>
       </c>
       <c r="H21" t="n">
-        <v>23.2163735324878</v>
+        <v>34.37861092145651</v>
       </c>
       <c r="I21" t="n">
-        <v>539</v>
+        <v>1181.888888888889</v>
       </c>
       <c r="J21" t="n">
-        <v>52.5</v>
+        <v>61.33333333333334</v>
       </c>
       <c r="K21" t="n">
-        <v>27.5</v>
+        <v>12.28368384845885</v>
       </c>
       <c r="L21" t="n">
-        <v>756.25</v>
+        <v>150.8888888888889</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.3</t>
+          <t>ProductGroup.TWO.4</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>256</v>
+        <v>172</v>
       </c>
       <c r="D22" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1360,82 +1360,82 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>43.5</v>
+        <v>40</v>
       </c>
       <c r="H22" t="n">
-        <v>26.7348087705897</v>
+        <v>28.5657137141714</v>
       </c>
       <c r="I22" t="n">
-        <v>714.75</v>
+        <v>816</v>
       </c>
       <c r="J22" t="n">
-        <v>354.5</v>
+        <v>49.5</v>
       </c>
       <c r="K22" t="n">
-        <v>59.5</v>
+        <v>27.5</v>
       </c>
       <c r="L22" t="n">
-        <v>3540.25</v>
+        <v>756.25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.1</t>
+          <t>ProductGroup.SIX.4</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="D23" t="n">
-        <v>7.969465648854962</v>
+        <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3481451679692024</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1212050579803042</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>23.2</v>
+        <v>42.66666666666666</v>
       </c>
       <c r="H23" t="n">
-        <v>19.62039754948916</v>
+        <v>46.91363222869115</v>
       </c>
       <c r="I23" t="n">
-        <v>384.96</v>
+        <v>2200.888888888889</v>
       </c>
       <c r="J23" t="n">
-        <v>87.5</v>
+        <v>80</v>
       </c>
       <c r="K23" t="n">
-        <v>45.5</v>
+        <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>2070.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.4</t>
+          <t>ProductGroup.TWELVE.4</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>564</v>
+        <v>156</v>
       </c>
       <c r="D24" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1444,40 +1444,40 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>57.81818181818182</v>
+        <v>36</v>
       </c>
       <c r="H24" t="n">
-        <v>19.49274075518269</v>
+        <v>26.15339366124404</v>
       </c>
       <c r="I24" t="n">
-        <v>379.9669421487604</v>
+        <v>684</v>
       </c>
       <c r="J24" t="n">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="K24" t="n">
-        <v>1.632993161855452</v>
+        <v>22</v>
       </c>
       <c r="L24" t="n">
-        <v>2.666666666666667</v>
+        <v>484</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.2</t>
+          <t>ProductGroup.TEN.4</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D25" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1486,40 +1486,40 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H25" t="n">
-        <v>18.49324200890693</v>
+        <v>24.55605831561735</v>
       </c>
       <c r="I25" t="n">
-        <v>342</v>
+        <v>603</v>
       </c>
       <c r="J25" t="n">
-        <v>700</v>
+        <v>131</v>
       </c>
       <c r="K25" t="n">
-        <v>668</v>
+        <v>56</v>
       </c>
       <c r="L25" t="n">
-        <v>446224</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.3</t>
+          <t>ProductGroup.ELEVEN.4</t>
         </is>
       </c>
       <c r="C26" t="n">
         <v>36</v>
       </c>
       <c r="D26" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1528,40 +1528,40 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H26" t="n">
-        <v>31.51190251317746</v>
+        <v>27.44084546802449</v>
       </c>
       <c r="I26" t="n">
-        <v>993</v>
+        <v>753</v>
       </c>
       <c r="J26" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="K26" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.3</t>
+          <t>ProductGroup.FOUR.1</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D27" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -1570,40 +1570,40 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H27" t="n">
-        <v>18</v>
+        <v>25.15949125081825</v>
       </c>
       <c r="I27" t="n">
-        <v>324</v>
+        <v>633</v>
       </c>
       <c r="J27" t="n">
-        <v>35.5</v>
+        <v>32.5</v>
       </c>
       <c r="K27" t="n">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="L27" t="n">
-        <v>42.25</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.3</t>
+          <t>ProductGroup.ONE.2</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="D28" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1612,40 +1612,40 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>37.5</v>
+        <v>54.28571428571428</v>
       </c>
       <c r="H28" t="n">
-        <v>37.55995207664674</v>
+        <v>45.41149724059594</v>
       </c>
       <c r="I28" t="n">
-        <v>1410.75</v>
+        <v>2062.204081632653</v>
       </c>
       <c r="J28" t="n">
-        <v>34.5</v>
+        <v>44.5</v>
       </c>
       <c r="K28" t="n">
-        <v>6.5</v>
+        <v>21.5</v>
       </c>
       <c r="L28" t="n">
-        <v>42.25</v>
+        <v>462.25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.3</t>
+          <t>ProductGroup.TWO.3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>48</v>
+        <v>352</v>
       </c>
       <c r="D29" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1654,40 +1654,40 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>61.5</v>
+        <v>37</v>
       </c>
       <c r="H29" t="n">
-        <v>57.19047123428867</v>
+        <v>25.45977219065403</v>
       </c>
       <c r="I29" t="n">
-        <v>3270.75</v>
+        <v>648.2</v>
       </c>
       <c r="J29" t="n">
-        <v>28.5</v>
+        <v>180</v>
       </c>
       <c r="K29" t="n">
-        <v>14.5</v>
+        <v>197.9966329680044</v>
       </c>
       <c r="L29" t="n">
-        <v>210.25</v>
+        <v>39202.66666666666</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.2</t>
+          <t>ProductGroup.TWELVE.3</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="D30" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -1696,40 +1696,40 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>24</v>
+        <v>16.5</v>
       </c>
       <c r="H30" t="n">
-        <v>24.16609194718914</v>
+        <v>16.51514456491374</v>
       </c>
       <c r="I30" t="n">
-        <v>584</v>
+        <v>272.75</v>
       </c>
       <c r="J30" t="n">
-        <v>1014.5</v>
+        <v>43</v>
       </c>
       <c r="K30" t="n">
-        <v>715.5</v>
+        <v>3</v>
       </c>
       <c r="L30" t="n">
-        <v>511940.25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.1</t>
+          <t>ProductGroup.SEVEN.3</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>20</v>
+        <v>696</v>
       </c>
       <c r="D31" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1738,40 +1738,40 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H31" t="n">
-        <v>52.3354564325181</v>
+        <v>18.38477631085023</v>
       </c>
       <c r="I31" t="n">
-        <v>2739</v>
+        <v>338</v>
       </c>
       <c r="J31" t="n">
-        <v>346.5</v>
+        <v>40.5</v>
       </c>
       <c r="K31" t="n">
-        <v>218.5</v>
+        <v>0.5</v>
       </c>
       <c r="L31" t="n">
-        <v>47742.25</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.3</t>
+          <t>ProductGroup.SIX.2</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D32" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1780,79 +1780,79 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>54.66666666666666</v>
+        <v>24</v>
       </c>
       <c r="H32" t="n">
-        <v>58.11100488624241</v>
+        <v>24</v>
       </c>
       <c r="I32" t="n">
-        <v>3376.888888888889</v>
+        <v>576</v>
       </c>
       <c r="J32" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="K32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.1</t>
+          <t>ProductGroup.THREE.1</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>51</v>
+        <v>152</v>
       </c>
       <c r="D33" t="n">
-        <v>7.941176470588236</v>
+        <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>0.4159451654038515</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1730103806228374</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>24</v>
+        <v>27.33333333333333</v>
       </c>
       <c r="H33" t="n">
-        <v>16.97056274847714</v>
+        <v>32.59175083088085</v>
       </c>
       <c r="I33" t="n">
-        <v>288</v>
+        <v>1062.222222222222</v>
       </c>
       <c r="J33" t="n">
-        <v>444</v>
+        <v>380.6666666666667</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>481.7781877817034</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>232110.2222222222</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Ma: 0, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.4</t>
+          <t>ProductGroup.FOURTEEN.3</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="D34" t="n">
         <v>10</v>
@@ -1864,37 +1864,37 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>30</v>
+        <v>22.66666666666667</v>
       </c>
       <c r="H34" t="n">
-        <v>30</v>
+        <v>23.87932625142975</v>
       </c>
       <c r="I34" t="n">
-        <v>900</v>
+        <v>570.2222222222222</v>
       </c>
       <c r="J34" t="n">
-        <v>43</v>
+        <v>34.66666666666666</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>6.847546194724712</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>46.88888888888889</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ProductGroup.FOURTEEN.1</t>
+          <t>ProductGroup.TEN.1</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="D35" t="n">
         <v>10</v>
@@ -1906,40 +1906,40 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="H35" t="n">
-        <v>55</v>
+        <v>22.20360331117452</v>
       </c>
       <c r="I35" t="n">
-        <v>3025</v>
+        <v>493</v>
       </c>
       <c r="J35" t="n">
-        <v>24</v>
+        <v>136.6666666666667</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>122.7391090438939</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>15064.88888888889</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.3</t>
+          <t>ProductGroup.ELEVEN.1</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D36" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1948,40 +1948,40 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H36" t="n">
-        <v>34</v>
+        <v>30.10537050649491</v>
       </c>
       <c r="I36" t="n">
-        <v>1156</v>
+        <v>906.3333333333334</v>
       </c>
       <c r="J36" t="n">
-        <v>23</v>
+        <v>31.66666666666667</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>9.428090415820632</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>88.88888888888887</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.1</t>
+          <t>ProductGroup.TWELVE.3</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>356</v>
+        <v>92</v>
       </c>
       <c r="D37" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1990,40 +1990,40 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H37" t="n">
-        <v>25.79922479455536</v>
+        <v>14</v>
       </c>
       <c r="I37" t="n">
-        <v>665.6</v>
+        <v>196</v>
       </c>
       <c r="J37" t="n">
-        <v>36</v>
+        <v>1787</v>
       </c>
       <c r="K37" t="n">
-        <v>11.7756811551038</v>
+        <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>138.6666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.1</t>
+          <t>ProductGroup.SEVEN.3</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>210</v>
+        <v>564</v>
       </c>
       <c r="D38" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -2032,40 +2032,40 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>39.5</v>
+        <v>17</v>
       </c>
       <c r="H38" t="n">
-        <v>26.32014437650371</v>
+        <v>17</v>
       </c>
       <c r="I38" t="n">
-        <v>692.75</v>
+        <v>289</v>
       </c>
       <c r="J38" t="n">
-        <v>477</v>
+        <v>124.3333333333333</v>
       </c>
       <c r="K38" t="n">
-        <v>455</v>
+        <v>151.7944516626202</v>
       </c>
       <c r="L38" t="n">
-        <v>207025</v>
+        <v>23041.55555555556</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.3</t>
+          <t>ProductGroup.FOUR.1</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D39" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -2074,16 +2074,16 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="J39" t="n">
-        <v>167</v>
+        <v>21</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
@@ -2095,19 +2095,19 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ProductGroup.TWELVE.3</t>
+          <t>ProductGroup.EIGHT.3</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="D40" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -2116,40 +2116,40 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>14</v>
+        <v>53.33333333333334</v>
       </c>
       <c r="H40" t="n">
-        <v>14</v>
+        <v>50.38077234642421</v>
       </c>
       <c r="I40" t="n">
-        <v>196</v>
+        <v>2538.222222222222</v>
       </c>
       <c r="J40" t="n">
-        <v>1771</v>
+        <v>51.5</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.1</t>
+          <t>ProductGroup.FOUR.2</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="D41" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -2158,40 +2158,40 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>44</v>
+        <v>32.25</v>
       </c>
       <c r="H41" t="n">
-        <v>44</v>
+        <v>27.43059423344671</v>
       </c>
       <c r="I41" t="n">
-        <v>1936</v>
+        <v>752.4375</v>
       </c>
       <c r="J41" t="n">
-        <v>21</v>
+        <v>41.66666666666666</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>0.9428090415820634</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>0.888888888888889</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.3</t>
+          <t>ProductGroup.FOURTEEN.1</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>564</v>
+        <v>4</v>
       </c>
       <c r="D42" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -2200,16 +2200,16 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H42" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I42" t="n">
-        <v>289</v>
+        <v>441</v>
       </c>
       <c r="J42" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
@@ -2221,16 +2221,16 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.4</t>
+          <t>ProductGroup.ONE.3</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>180</v>
+        <v>48</v>
       </c>
       <c r="D43" t="n">
         <v>8</v>
@@ -2242,37 +2242,37 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>47.33333333333334</v>
+        <v>77.5</v>
       </c>
       <c r="H43" t="n">
-        <v>21.31248981752771</v>
+        <v>69.67603605257693</v>
       </c>
       <c r="I43" t="n">
-        <v>454.2222222222222</v>
+        <v>4854.75</v>
       </c>
       <c r="J43" t="n">
-        <v>44</v>
+        <v>47.5</v>
       </c>
       <c r="K43" t="n">
-        <v>2</v>
+        <v>7.5</v>
       </c>
       <c r="L43" t="n">
-        <v>4</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.4</t>
+          <t>ProductGroup.TWO.2</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>16</v>
+        <v>352</v>
       </c>
       <c r="D44" t="n">
         <v>8</v>
@@ -2284,37 +2284,37 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>29</v>
+        <v>37.625</v>
       </c>
       <c r="H44" t="n">
-        <v>29</v>
+        <v>20.22645235823623</v>
       </c>
       <c r="I44" t="n">
-        <v>841</v>
+        <v>409.109375</v>
       </c>
       <c r="J44" t="n">
-        <v>44</v>
+        <v>630</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>1035.190079164208</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>1071618.5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ProductGroup.FIFTEEN.4</t>
+          <t>ProductGroup.THREE.3</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="D45" t="n">
         <v>8</v>
@@ -2326,37 +2326,37 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>21</v>
+        <v>45.55555555555556</v>
       </c>
       <c r="H45" t="n">
-        <v>21</v>
+        <v>47.42974011012057</v>
       </c>
       <c r="I45" t="n">
-        <v>441</v>
+        <v>2249.58024691358</v>
       </c>
       <c r="J45" t="n">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>20.11632835948615</v>
       </c>
       <c r="L45" t="n">
-        <v>0</v>
+        <v>404.6666666666667</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.4</t>
+          <t>ProductGroup.ELEVEN.3</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
@@ -2368,37 +2368,37 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>85.33333333333333</v>
+        <v>20.33333333333333</v>
       </c>
       <c r="H46" t="n">
-        <v>77.72315542287825</v>
+        <v>21.30466824169973</v>
       </c>
       <c r="I46" t="n">
-        <v>6040.888888888888</v>
+        <v>453.8888888888889</v>
       </c>
       <c r="J46" t="n">
-        <v>88</v>
+        <v>41.33333333333334</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>13.22455628325158</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>174.8888888888889</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.4</t>
+          <t>ProductGroup.SIX.1</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D47" t="n">
         <v>8</v>
@@ -2410,16 +2410,16 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>39.33333333333334</v>
+        <v>21</v>
       </c>
       <c r="H47" t="n">
-        <v>27.82484900627894</v>
+        <v>21</v>
       </c>
       <c r="I47" t="n">
-        <v>774.2222222222223</v>
+        <v>441</v>
       </c>
       <c r="J47" t="n">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="K47" t="n">
         <v>0</v>
@@ -2431,16 +2431,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.4</t>
+          <t>ProductGroup.FIFTEEN.3</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D48" t="n">
         <v>8</v>
@@ -2452,37 +2452,37 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>57.6</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="H48" t="n">
-        <v>47.58823383988946</v>
+        <v>43.15347288715269</v>
       </c>
       <c r="I48" t="n">
-        <v>2264.64</v>
+        <v>1862.222222222222</v>
       </c>
       <c r="J48" t="n">
-        <v>85</v>
+        <v>44.33333333333334</v>
       </c>
       <c r="K48" t="n">
-        <v>0</v>
+        <v>8.178562764256865</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>66.88888888888889</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ProductGroup.ELEVEN.4</t>
+          <t>ProductGroup.THIRTEEN.1</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D49" t="n">
         <v>8</v>
@@ -2494,16 +2494,16 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H49" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I49" t="n">
-        <v>1089</v>
+        <v>441</v>
       </c>
       <c r="J49" t="n">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="K49" t="n">
         <v>0</v>
@@ -2515,19 +2515,19 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ProductGroup.THREE.2</t>
+          <t>ProductGroup.TWO.4</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D50" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -2536,37 +2536,37 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>27.33333333333333</v>
+        <v>55.25</v>
       </c>
       <c r="H50" t="n">
-        <v>38.6551707048646</v>
+        <v>24.1026450830609</v>
       </c>
       <c r="I50" t="n">
-        <v>1494.222222222222</v>
+        <v>580.9375</v>
       </c>
       <c r="J50" t="n">
-        <v>241.5</v>
+        <v>43.5</v>
       </c>
       <c r="K50" t="n">
-        <v>237.5</v>
+        <v>1.5</v>
       </c>
       <c r="L50" t="n">
-        <v>56406.25</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ProductGroup.TWO.1</t>
+          <t>ProductGroup.SEVEN.4</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>76</v>
+        <v>904</v>
       </c>
       <c r="D51" t="n">
         <v>8</v>
@@ -2578,37 +2578,37 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>32</v>
+        <v>54.63157894736842</v>
       </c>
       <c r="H51" t="n">
-        <v>32</v>
+        <v>18.76225361370057</v>
       </c>
       <c r="I51" t="n">
-        <v>1024</v>
+        <v>352.02216066482</v>
       </c>
       <c r="J51" t="n">
-        <v>177</v>
+        <v>44.7</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>6.067124524847006</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>36.81</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ProductGroup.NINE.3</t>
+          <t>ProductGroup.THREE.4</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="D52" t="n">
         <v>8</v>
@@ -2620,33 +2620,33 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H52" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="I52" t="n">
-        <v>324</v>
+        <v>1089</v>
       </c>
       <c r="J52" t="n">
-        <v>85.5</v>
+        <v>82</v>
       </c>
       <c r="K52" t="n">
-        <v>39.5</v>
+        <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>1560.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ProductGroup.FOUR.3</t>
+          <t>ProductGroup.ONE.4</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -2662,16 +2662,16 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>50</v>
+        <v>45.33333333333334</v>
       </c>
       <c r="H53" t="n">
-        <v>42.55192905928786</v>
+        <v>32.71425105702746</v>
       </c>
       <c r="I53" t="n">
-        <v>1810.666666666667</v>
+        <v>1070.222222222222</v>
       </c>
       <c r="J53" t="n">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="K53" t="n">
         <v>0</v>
@@ -2683,16 +2683,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ProductGroup.ONE.1</t>
+          <t>ProductGroup.NINE.4</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D54" t="n">
         <v>8</v>
@@ -2704,37 +2704,37 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>20.5</v>
+        <v>43</v>
       </c>
       <c r="H54" t="n">
-        <v>20.80264406271472</v>
+        <v>24.87971060924946</v>
       </c>
       <c r="I54" t="n">
-        <v>432.75</v>
+        <v>619</v>
       </c>
       <c r="J54" t="n">
-        <v>37.5</v>
+        <v>81</v>
       </c>
       <c r="K54" t="n">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="L54" t="n">
-        <v>72.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ProductGroup.THIRTEEN.3</t>
+          <t>ProductGroup.FOUR.4</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D55" t="n">
         <v>8</v>
@@ -2746,16 +2746,16 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>65</v>
+        <v>38.66666666666666</v>
       </c>
       <c r="H55" t="n">
-        <v>65</v>
+        <v>29.04402788105595</v>
       </c>
       <c r="I55" t="n">
-        <v>4225</v>
+        <v>843.5555555555555</v>
       </c>
       <c r="J55" t="n">
-        <v>224</v>
+        <v>48</v>
       </c>
       <c r="K55" t="n">
         <v>0</v>
@@ -2767,37 +2767,37 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.1</t>
+          <t>ProductGroup.FIFTEEN.4</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D56" t="n">
-        <v>7.8</v>
+        <v>8</v>
       </c>
       <c r="E56" t="n">
-        <v>1.077032961426901</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>1.16</v>
+        <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>1156</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="K56" t="n">
         <v>0</v>
@@ -2809,16 +2809,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ProductGroup.TEN.3</t>
+          <t>ProductGroup.TWELVE.4</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="D57" t="n">
         <v>8</v>
@@ -2830,37 +2830,37 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>33.66666666666666</v>
+        <v>64.8</v>
       </c>
       <c r="H57" t="n">
-        <v>25.70127536826831</v>
+        <v>39.77134646953759</v>
       </c>
       <c r="I57" t="n">
-        <v>660.5555555555555</v>
+        <v>1581.76</v>
       </c>
       <c r="J57" t="n">
-        <v>223</v>
+        <v>82</v>
       </c>
       <c r="K57" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>30625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ProductGroup.EIGHT.1</t>
+          <t>ProductGroup.TEN.4</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D58" t="n">
         <v>8</v>
@@ -2872,40 +2872,40 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>19</v>
+        <v>34.5</v>
       </c>
       <c r="H58" t="n">
-        <v>19.05255888325765</v>
+        <v>24.05722344743882</v>
       </c>
       <c r="I58" t="n">
-        <v>363</v>
+        <v>578.75</v>
       </c>
       <c r="J58" t="n">
-        <v>97</v>
+        <v>330</v>
       </c>
       <c r="K58" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="L58" t="n">
-        <v>4225</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Ma: 1, 1</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ProductGroup.SEVEN.1</t>
+          <t>ProductGroup.ELEVEN.4</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>564</v>
+        <v>28</v>
       </c>
       <c r="D59" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -2914,22 +2914,190 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>26.57142857142857</v>
+        <v>37</v>
       </c>
       <c r="H59" t="n">
-        <v>13.92692297937593</v>
+        <v>37</v>
       </c>
       <c r="I59" t="n">
-        <v>193.9591836734694</v>
+        <v>1369</v>
       </c>
       <c r="J59" t="n">
-        <v>101.3</v>
+        <v>82</v>
       </c>
       <c r="K59" t="n">
-        <v>263.3904136448402</v>
+        <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>69374.51000000001</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Ma: 3, 1</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOURTEEN.1</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>40</v>
+      </c>
+      <c r="D60" t="n">
+        <v>10</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>16</v>
+      </c>
+      <c r="H60" t="n">
+        <v>16</v>
+      </c>
+      <c r="I60" t="n">
+        <v>256</v>
+      </c>
+      <c r="J60" t="n">
+        <v>24</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ProductGroup.FOURTEEN.1</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>16</v>
+      </c>
+      <c r="D61" t="n">
+        <v>10</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>18</v>
+      </c>
+      <c r="H61" t="n">
+        <v>18</v>
+      </c>
+      <c r="I61" t="n">
+        <v>324</v>
+      </c>
+      <c r="J61" t="n">
+        <v>50</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ProductGroup.EIGHT.3</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>12</v>
+      </c>
+      <c r="D62" t="n">
+        <v>10</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>40</v>
+      </c>
+      <c r="H62" t="n">
+        <v>40</v>
+      </c>
+      <c r="I62" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J62" t="n">
+        <v>28</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Ma: 3, 2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>ProductGroup.THIRTEEN.1</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>20</v>
+      </c>
+      <c r="D63" t="n">
+        <v>10</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>42</v>
+      </c>
+      <c r="H63" t="n">
+        <v>47.05316142407437</v>
+      </c>
+      <c r="I63" t="n">
+        <v>2214</v>
+      </c>
+      <c r="J63" t="n">
+        <v>29</v>
+      </c>
+      <c r="K63" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2943,7 +3111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3011,14 +3179,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ma: 0, 4</t>
+          <t>Ma: 1, 2</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>964</v>
+        <v>1712</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -3027,72 +3195,72 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>31.8</v>
+        <v>30.25396825396825</v>
       </c>
       <c r="G2" t="n">
-        <v>29.28412539243746</v>
+        <v>30.51617747077054</v>
       </c>
       <c r="H2" t="n">
-        <v>857.5600000000004</v>
+        <v>931.2370874275636</v>
       </c>
       <c r="I2" t="n">
-        <v>142.25</v>
+        <v>252.4615384615385</v>
       </c>
       <c r="J2" t="n">
-        <v>157.7351815544015</v>
+        <v>835.5947780689482</v>
       </c>
       <c r="K2" t="n">
-        <v>24880.3875</v>
+        <v>698218.6331360948</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ma: 2, 2</t>
+          <t>Ma: 1, 1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1127</v>
+        <v>564</v>
       </c>
       <c r="C3" t="n">
-        <v>7.996450754214729</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1190982199507543</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01418438599543826</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>34.23255813953488</v>
+        <v>25.42857142857143</v>
       </c>
       <c r="G3" t="n">
-        <v>29.15303423460119</v>
+        <v>12.86031706848788</v>
       </c>
       <c r="H3" t="n">
-        <v>849.8994050838287</v>
+        <v>165.3877551020408</v>
       </c>
       <c r="I3" t="n">
-        <v>160.1875</v>
+        <v>93.18181818181819</v>
       </c>
       <c r="J3" t="n">
-        <v>221.5643864517716</v>
+        <v>253.5448026328853</v>
       </c>
       <c r="K3" t="n">
-        <v>49090.77734375</v>
+        <v>64284.96694214876</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ma: 0, 3</t>
+          <t>Ma: 0, 1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>564</v>
+        <v>1284</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -3101,69 +3269,69 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>57.81818181818182</v>
+        <v>33.67164179104478</v>
       </c>
       <c r="G4" t="n">
-        <v>19.49274075518269</v>
+        <v>30.81693082808103</v>
       </c>
       <c r="H4" t="n">
-        <v>379.9669421487604</v>
+        <v>949.6832256627312</v>
       </c>
       <c r="I4" t="n">
-        <v>46</v>
+        <v>73.45161290322581</v>
       </c>
       <c r="J4" t="n">
-        <v>1.632993161855452</v>
+        <v>39.62065175871846</v>
       </c>
       <c r="K4" t="n">
-        <v>2.666666666666667</v>
+        <v>1569.79604578564</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ma: 3, 2</t>
+          <t>Ma: 2, 2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>663</v>
+        <v>1688</v>
       </c>
       <c r="C5" t="n">
-        <v>7.995475113122172</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1164224464277702</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01355418603222702</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>38.29268292682926</v>
+        <v>30.50847457627119</v>
       </c>
       <c r="G5" t="n">
-        <v>45.19564186978005</v>
+        <v>29.9730799452091</v>
       </c>
       <c r="H5" t="n">
-        <v>2042.646044021416</v>
+        <v>898.385521401896</v>
       </c>
       <c r="I5" t="n">
-        <v>288.0588235294118</v>
+        <v>110.5</v>
       </c>
       <c r="J5" t="n">
-        <v>490.4157264761057</v>
+        <v>221.4318932162513</v>
       </c>
       <c r="K5" t="n">
-        <v>240507.5847750866</v>
+        <v>49032.08333333334</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ma: 0, 1</t>
+          <t>Ma: 2, 1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92</v>
+        <v>708</v>
       </c>
       <c r="C6" t="n">
         <v>10</v>
@@ -3175,35 +3343,35 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G6" t="n">
-        <v>30</v>
+        <v>15.13274595042156</v>
       </c>
       <c r="H6" t="n">
-        <v>900</v>
+        <v>229</v>
       </c>
       <c r="I6" t="n">
-        <v>43</v>
+        <v>436.2</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>686.7253890748469</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>471591.76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ma: 3, 1</t>
+          <t>Ma: 3, 3</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>40</v>
+        <v>784</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -3212,35 +3380,35 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>55</v>
+        <v>41.07692307692308</v>
       </c>
       <c r="G7" t="n">
-        <v>55</v>
+        <v>43.16847414217133</v>
       </c>
       <c r="H7" t="n">
-        <v>3025</v>
+        <v>1863.517159763315</v>
       </c>
       <c r="I7" t="n">
-        <v>24</v>
+        <v>147.695652173913</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>485.2891056556421</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>235505.5160680529</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ma: 1, 2</t>
+          <t>Ma: 0, 2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>626</v>
+        <v>180</v>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -3249,35 +3417,35 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>36.33333333333334</v>
+        <v>55.25</v>
       </c>
       <c r="G8" t="n">
-        <v>28.78464096624371</v>
+        <v>24.1026450830609</v>
       </c>
       <c r="H8" t="n">
-        <v>828.5555555555555</v>
+        <v>580.9375</v>
       </c>
       <c r="I8" t="n">
-        <v>178.8571428571429</v>
+        <v>43.5</v>
       </c>
       <c r="J8" t="n">
-        <v>311.1960468769433</v>
+        <v>1.5</v>
       </c>
       <c r="K8" t="n">
-        <v>96842.97959183672</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ma: 2, 1</t>
+          <t>Ma: 0, 3</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>680</v>
+        <v>1176</v>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -3286,35 +3454,35 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>25</v>
+        <v>48.45454545454545</v>
       </c>
       <c r="G9" t="n">
-        <v>31.44837038703277</v>
+        <v>28.91637987012531</v>
       </c>
       <c r="H9" t="n">
-        <v>989</v>
+        <v>836.1570247933884</v>
       </c>
       <c r="I9" t="n">
-        <v>608.3333333333334</v>
+        <v>73.16666666666667</v>
       </c>
       <c r="J9" t="n">
-        <v>822.1440803708854</v>
+        <v>64.78104146533407</v>
       </c>
       <c r="K9" t="n">
-        <v>675920.8888888889</v>
+        <v>4196.583333333332</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ma: 0, 2</t>
+          <t>Ma: 3, 1</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>324</v>
+        <v>40</v>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -3323,96 +3491,59 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>48.34782608695652</v>
+        <v>16</v>
       </c>
       <c r="G10" t="n">
-        <v>45.07636872035315</v>
+        <v>16</v>
       </c>
       <c r="H10" t="n">
-        <v>2031.879017013232</v>
+        <v>256</v>
       </c>
       <c r="I10" t="n">
-        <v>62.125</v>
+        <v>24</v>
       </c>
       <c r="J10" t="n">
-        <v>20.40488605702075</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>416.359375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ma: 1, 3</t>
+          <t>Ma: 3, 2</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>538</v>
+        <v>48</v>
       </c>
       <c r="C11" t="n">
-        <v>7.988847583643123</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2584378489127825</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0667901217506662</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>31.93103448275862</v>
+        <v>35.5</v>
       </c>
       <c r="G11" t="n">
-        <v>34.92448112268049</v>
+        <v>41.11873052515119</v>
       </c>
       <c r="H11" t="n">
-        <v>1219.719381688466</v>
+        <v>1690.75</v>
       </c>
       <c r="I11" t="n">
-        <v>138.3846153846154</v>
+        <v>34</v>
       </c>
       <c r="J11" t="n">
-        <v>144.5212459555493</v>
+        <v>9.273618495495704</v>
       </c>
       <c r="K11" t="n">
-        <v>20886.39053254438</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Ma: 1, 1</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>564</v>
-      </c>
-      <c r="C12" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>26.57142857142857</v>
-      </c>
-      <c r="G12" t="n">
-        <v>13.92692297937593</v>
-      </c>
-      <c r="H12" t="n">
-        <v>193.9591836734694</v>
-      </c>
-      <c r="I12" t="n">
-        <v>101.3</v>
-      </c>
-      <c r="J12" t="n">
-        <v>263.3904136448402</v>
-      </c>
-      <c r="K12" t="n">
-        <v>69374.51000000001</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>